<commit_message>
Published state of ETDataset on 17 April 2015
</commit_message>
<xml_diff>
--- a/nodes_source_analyses/energy/energy_chp_supercritical_waste_mix.central_producer.xlsx
+++ b/nodes_source_analyses/energy/energy_chp_supercritical_waste_mix.central_producer.xlsx
@@ -211,9 +211,6 @@
     <t>This sheet summarizes all node attributes formatted in the way they are used by the Energy Transition Model. Use the Excel formulas to find the original data and sources for these numbers. You can also use this document to update the attribute value. Once you have finished updating, save this document and use the button to update the node attributes on ETSource.</t>
   </si>
   <si>
-    <t>energy_chp_supercritical_waste_mix.central.producer.ad</t>
-  </si>
-  <si>
     <t>ccs_investment</t>
   </si>
   <si>
@@ -823,14 +820,17 @@
   <si>
     <t>http://refman.et-model.com/publications/1937</t>
   </si>
+  <si>
+    <t>energy_chp_supercritical_waste_mix.central_producer.ad</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="24" x14ac:knownFonts="1">
     <font>
@@ -1660,15 +1660,15 @@
     <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="11" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="11" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1679,15 +1679,15 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="7" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="227" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="227" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1748,18 +1748,18 @@
     <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="227" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="165" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="49" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1767,7 +1767,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1784,7 +1784,7 @@
     <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2837,7 +2837,9 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -2859,7 +2861,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>55</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="2:3" s="49" customFormat="1">
@@ -3123,7 +3125,7 @@
     <row r="12" spans="2:11" ht="16" thickBot="1">
       <c r="B12" s="21"/>
       <c r="C12" s="29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>34</v>
@@ -3134,7 +3136,7 @@
       </c>
       <c r="F12" s="24"/>
       <c r="G12" s="64" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H12" s="24"/>
       <c r="I12" s="25" t="s">
@@ -3146,7 +3148,7 @@
     <row r="13" spans="2:11" ht="16" thickBot="1">
       <c r="B13" s="21"/>
       <c r="C13" s="64" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>2</v>
@@ -3167,7 +3169,7 @@
     <row r="14" spans="2:11" ht="16" thickBot="1">
       <c r="B14" s="21"/>
       <c r="C14" s="64" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>2</v>
@@ -3188,7 +3190,7 @@
     <row r="15" spans="2:11" ht="16" thickBot="1">
       <c r="B15" s="21"/>
       <c r="C15" s="64" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>2</v>
@@ -3208,7 +3210,7 @@
     <row r="16" spans="2:11" ht="16" thickBot="1">
       <c r="B16" s="21"/>
       <c r="C16" s="64" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>2</v>
@@ -3228,7 +3230,7 @@
     <row r="17" spans="2:11" ht="16" thickBot="1">
       <c r="B17" s="21"/>
       <c r="C17" s="64" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>2</v>
@@ -3248,7 +3250,7 @@
     <row r="18" spans="2:11" ht="16" thickBot="1">
       <c r="B18" s="21"/>
       <c r="C18" s="64" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>2</v>
@@ -3268,7 +3270,7 @@
     <row r="19" spans="2:11" ht="16" thickBot="1">
       <c r="B19" s="21"/>
       <c r="C19" s="64" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>2</v>
@@ -3288,7 +3290,7 @@
     <row r="20" spans="2:11" ht="16" thickBot="1">
       <c r="B20" s="21"/>
       <c r="C20" s="64" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>2</v>
@@ -3308,7 +3310,7 @@
     <row r="21" spans="2:11" ht="16" thickBot="1">
       <c r="B21" s="21"/>
       <c r="C21" s="64" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>2</v>
@@ -3318,7 +3320,7 @@
       </c>
       <c r="F21" s="24"/>
       <c r="G21" s="72" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H21" s="24"/>
       <c r="I21" s="70" t="s">
@@ -3330,7 +3332,7 @@
     <row r="22" spans="2:11" ht="16" thickBot="1">
       <c r="B22" s="21"/>
       <c r="C22" s="64" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>2</v>
@@ -3340,7 +3342,7 @@
       </c>
       <c r="F22" s="24"/>
       <c r="G22" s="64" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H22" s="24"/>
       <c r="I22" s="70" t="s">
@@ -3352,7 +3354,7 @@
     <row r="23" spans="2:11" ht="16" thickBot="1">
       <c r="B23" s="21"/>
       <c r="C23" s="64" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>2</v>
@@ -3362,7 +3364,7 @@
       </c>
       <c r="F23" s="24"/>
       <c r="G23" s="64" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H23" s="24"/>
       <c r="I23" s="70" t="s">
@@ -3374,7 +3376,7 @@
     <row r="24" spans="2:11" ht="16" thickBot="1">
       <c r="B24" s="21"/>
       <c r="C24" s="64" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>2</v>
@@ -3384,7 +3386,7 @@
       </c>
       <c r="F24" s="24"/>
       <c r="G24" s="64" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H24" s="24"/>
       <c r="I24" s="70" t="s">
@@ -3396,7 +3398,7 @@
     <row r="25" spans="2:11" ht="16" thickBot="1">
       <c r="B25" s="21"/>
       <c r="C25" s="64" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>2</v>
@@ -3406,7 +3408,7 @@
       </c>
       <c r="F25" s="24"/>
       <c r="G25" s="135" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H25" s="24"/>
       <c r="I25" s="25" t="s">
@@ -3447,7 +3449,7 @@
         <v>25</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E28" s="41">
         <f>'Research data'!F19</f>
@@ -3459,7 +3461,7 @@
       </c>
       <c r="H28" s="24"/>
       <c r="I28" s="87" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J28" s="22"/>
       <c r="K28" s="14"/>
@@ -3467,17 +3469,17 @@
     <row r="29" spans="2:11" ht="16" thickBot="1">
       <c r="B29" s="21"/>
       <c r="C29" s="64" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E29" s="41">
         <v>0</v>
       </c>
       <c r="F29" s="24"/>
       <c r="G29" s="64" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H29" s="24"/>
       <c r="I29" s="25" t="s">
@@ -3492,14 +3494,14 @@
         <v>26</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E30" s="66">
         <v>0</v>
       </c>
       <c r="F30" s="24"/>
       <c r="G30" s="64" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H30" s="24"/>
       <c r="I30" s="25" t="s">
@@ -3511,17 +3513,17 @@
     <row r="31" spans="2:11" ht="16" thickBot="1">
       <c r="B31" s="21"/>
       <c r="C31" s="64" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E31" s="66">
         <v>0</v>
       </c>
       <c r="F31" s="24"/>
       <c r="G31" s="64" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H31" s="24"/>
       <c r="I31" s="25" t="s">
@@ -3533,10 +3535,10 @@
     <row r="32" spans="2:11" ht="16" thickBot="1">
       <c r="B32" s="21"/>
       <c r="C32" s="64" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E32" s="66">
         <f>'Research data'!F22</f>
@@ -3544,11 +3546,11 @@
       </c>
       <c r="F32" s="24"/>
       <c r="G32" s="64" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H32" s="24"/>
       <c r="I32" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J32" s="22"/>
       <c r="K32" s="14"/>
@@ -3556,21 +3558,21 @@
     <row r="33" spans="2:11" ht="16" thickBot="1">
       <c r="B33" s="21"/>
       <c r="C33" s="64" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E33" s="41">
         <v>0</v>
       </c>
       <c r="F33" s="24"/>
       <c r="G33" s="64" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H33" s="24"/>
       <c r="I33" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J33" s="22"/>
       <c r="K33" s="14"/>
@@ -3578,17 +3580,17 @@
     <row r="34" spans="2:11" ht="16" thickBot="1">
       <c r="B34" s="21"/>
       <c r="C34" s="64" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E34" s="41">
         <v>0</v>
       </c>
       <c r="F34" s="24"/>
       <c r="G34" s="64" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H34" s="24"/>
       <c r="I34" s="25" t="s">
@@ -3600,17 +3602,17 @@
     <row r="35" spans="2:11" ht="16" thickBot="1">
       <c r="B35" s="21"/>
       <c r="C35" s="65" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E35" s="68">
         <v>0.1</v>
       </c>
       <c r="F35" s="24"/>
       <c r="G35" s="24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H35" s="24"/>
       <c r="I35" s="25" t="s">
@@ -3622,10 +3624,10 @@
     <row r="36" spans="2:11" ht="16" thickBot="1">
       <c r="B36" s="21"/>
       <c r="C36" s="64" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E36" s="63">
         <v>1</v>
@@ -3668,7 +3670,7 @@
     <row r="39" spans="2:11" ht="16" thickBot="1">
       <c r="B39" s="21"/>
       <c r="C39" s="65" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>1</v>
@@ -3679,7 +3681,7 @@
       </c>
       <c r="F39" s="24"/>
       <c r="G39" s="64" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H39" s="24"/>
       <c r="I39" s="87" t="s">
@@ -3706,7 +3708,7 @@
       </c>
       <c r="H40" s="24"/>
       <c r="I40" s="87" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J40" s="22"/>
       <c r="K40" s="14"/>
@@ -3714,10 +3716,10 @@
     <row r="41" spans="2:11" ht="16" thickBot="1">
       <c r="B41" s="21"/>
       <c r="C41" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="D41" s="6" t="s">
         <v>75</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>76</v>
       </c>
       <c r="E41" s="63">
         <f>'Research data'!F14</f>
@@ -3725,11 +3727,11 @@
       </c>
       <c r="F41" s="24"/>
       <c r="G41" s="64" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H41" s="24"/>
       <c r="I41" s="87" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J41" s="22"/>
       <c r="K41" s="14"/>
@@ -3747,7 +3749,7 @@
       </c>
       <c r="F42" s="24"/>
       <c r="G42" s="64" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H42" s="24"/>
       <c r="I42" s="25" t="s">
@@ -3759,10 +3761,10 @@
     <row r="43" spans="2:11" ht="16" thickBot="1">
       <c r="B43" s="21"/>
       <c r="C43" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D43" s="134" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E43" s="124"/>
       <c r="F43" s="136"/>
@@ -3777,10 +3779,10 @@
     <row r="44" spans="2:11" ht="16" thickBot="1">
       <c r="B44" s="21"/>
       <c r="C44" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D44" s="134" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E44" s="127"/>
       <c r="F44" s="136"/>
@@ -3795,10 +3797,10 @@
     <row r="45" spans="2:11" ht="16" thickBot="1">
       <c r="B45" s="21"/>
       <c r="C45" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D45" s="134" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E45" s="125"/>
       <c r="F45" s="136"/>
@@ -3813,10 +3815,10 @@
     <row r="46" spans="2:11" ht="16" thickBot="1">
       <c r="B46" s="21"/>
       <c r="C46" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D46" s="134" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E46" s="127"/>
       <c r="F46" s="136"/>
@@ -3831,10 +3833,10 @@
     <row r="47" spans="2:11" ht="16" thickBot="1">
       <c r="B47" s="21"/>
       <c r="C47" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D47" s="134" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E47" s="126"/>
       <c r="F47" s="136"/>
@@ -3971,23 +3973,23 @@
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K3" s="4"/>
       <c r="L3" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M3" s="4"/>
       <c r="N3" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="O3" s="4"/>
       <c r="P3" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Q3" s="4"/>
       <c r="R3" s="4" t="s">
@@ -4064,7 +4066,7 @@
     <row r="7" spans="2:18" ht="16" thickBot="1">
       <c r="B7" s="75"/>
       <c r="C7" s="133" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D7" s="128" t="s">
         <v>34</v>
@@ -4090,10 +4092,10 @@
     <row r="8" spans="2:18" ht="16" thickBot="1">
       <c r="B8" s="75"/>
       <c r="C8" s="123" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D8" s="128" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E8" s="79"/>
       <c r="F8" s="80">
@@ -4119,10 +4121,10 @@
     <row r="9" spans="2:18" ht="16" thickBot="1">
       <c r="B9" s="75"/>
       <c r="C9" s="131" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D9" s="132" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E9" s="67"/>
       <c r="F9" s="129">
@@ -4173,7 +4175,7 @@
     <row r="12" spans="2:18" ht="16" thickBot="1">
       <c r="B12" s="75"/>
       <c r="C12" s="123" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D12" s="78" t="s">
         <v>1</v>
@@ -4205,7 +4207,7 @@
     <row r="13" spans="2:18" ht="16" thickBot="1">
       <c r="B13" s="75"/>
       <c r="C13" s="123" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D13" s="78" t="s">
         <v>1</v>
@@ -4234,10 +4236,10 @@
     <row r="14" spans="2:18" ht="16" thickBot="1">
       <c r="B14" s="75"/>
       <c r="C14" s="123" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D14" s="78" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E14" s="79"/>
       <c r="F14" s="82">
@@ -4262,7 +4264,7 @@
       </c>
       <c r="Q14" s="67"/>
       <c r="R14" s="83" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="2:18">
@@ -4277,7 +4279,7 @@
       <c r="P15" s="90"/>
       <c r="Q15" s="67"/>
       <c r="R15" s="84" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="2:18">
@@ -4298,7 +4300,7 @@
       <c r="P16" s="90"/>
       <c r="Q16" s="67"/>
       <c r="R16" s="84" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="2:18">
@@ -4344,10 +4346,10 @@
     <row r="19" spans="2:18" ht="16" thickBot="1">
       <c r="B19" s="75"/>
       <c r="C19" s="77" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D19" s="77" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E19" s="76"/>
       <c r="F19" s="80">
@@ -4376,7 +4378,7 @@
         <v>20</v>
       </c>
       <c r="D20" s="137" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E20" s="11"/>
       <c r="F20" s="80">
@@ -4397,16 +4399,16 @@
       <c r="P20" s="85"/>
       <c r="Q20" s="67"/>
       <c r="R20" s="142" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="2:18" ht="16" thickBot="1">
       <c r="B21" s="75"/>
       <c r="C21" s="138" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D21" s="77" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E21" s="11"/>
       <c r="F21" s="80">
@@ -4432,10 +4434,10 @@
     <row r="22" spans="2:18" ht="16" thickBot="1">
       <c r="B22" s="75"/>
       <c r="C22" s="91" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D22" s="77" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E22" s="92"/>
       <c r="F22" s="80">
@@ -4454,16 +4456,16 @@
       <c r="P22" s="67"/>
       <c r="Q22" s="67"/>
       <c r="R22" s="140" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="23" spans="2:18" ht="16" thickBot="1">
       <c r="B23" s="75"/>
       <c r="C23" s="91" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D23" s="138" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E23" s="92"/>
       <c r="F23" s="80">
@@ -4481,16 +4483,16 @@
       <c r="P23" s="67"/>
       <c r="Q23" s="67"/>
       <c r="R23" s="84" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="2:18" ht="16" thickBot="1">
       <c r="B24" s="75"/>
       <c r="C24" s="91" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D24" s="78" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E24" s="92"/>
       <c r="F24" s="80">
@@ -4512,10 +4514,10 @@
     <row r="25" spans="2:18" ht="16" thickBot="1">
       <c r="B25" s="75"/>
       <c r="C25" s="91" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D25" s="78" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E25" s="93"/>
       <c r="F25" s="80">
@@ -4537,10 +4539,10 @@
     <row r="26" spans="2:18" ht="16" thickBot="1">
       <c r="B26" s="75"/>
       <c r="C26" s="91" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D26" s="137" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E26" s="93"/>
       <c r="F26" s="80">
@@ -4562,10 +4564,10 @@
     <row r="27" spans="2:18" ht="16" thickBot="1">
       <c r="B27" s="75"/>
       <c r="C27" s="94" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D27" s="64" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E27" s="93"/>
       <c r="F27" s="80">
@@ -4587,10 +4589,10 @@
     <row r="28" spans="2:18" ht="16" thickBot="1">
       <c r="B28" s="75"/>
       <c r="C28" s="140" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D28" s="139" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E28" s="93"/>
       <c r="F28" s="80">
@@ -4716,13 +4718,13 @@
         <v>15</v>
       </c>
       <c r="H5" s="106" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I5" s="106" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J5" s="107" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K5" s="106" t="s">
         <v>8</v>
@@ -4745,10 +4747,10 @@
       <c r="C7" s="108"/>
       <c r="D7" s="108"/>
       <c r="E7" s="103" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F7" s="103" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G7" s="104" t="s">
         <v>21</v>
@@ -4758,16 +4760,16 @@
       </c>
       <c r="I7" s="104"/>
       <c r="J7" s="104" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K7" s="109" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="2:11">
       <c r="B8" s="100"/>
       <c r="C8" s="110" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D8" s="111"/>
       <c r="E8" s="103"/>
@@ -4795,7 +4797,7 @@
       <c r="C10" s="108"/>
       <c r="D10" s="108"/>
       <c r="E10" s="108" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F10" s="113" t="s">
         <v>22</v>
@@ -4804,20 +4806,20 @@
         <v>2000</v>
       </c>
       <c r="H10" s="114" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I10" s="115"/>
       <c r="J10" s="114" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K10" s="116" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="2:11">
       <c r="B11" s="100"/>
       <c r="C11" s="117" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D11" s="118"/>
       <c r="E11" s="108"/>
@@ -4845,20 +4847,20 @@
       <c r="C13" s="108"/>
       <c r="D13" s="108"/>
       <c r="E13" s="108" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F13" s="103" t="s">
         <v>5</v>
       </c>
       <c r="G13" s="104" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H13" s="104" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I13" s="104"/>
       <c r="J13" s="104" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K13" s="116"/>
     </row>
@@ -4879,7 +4881,7 @@
     <row r="15" spans="2:11">
       <c r="B15" s="100"/>
       <c r="C15" s="112" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D15" s="108"/>
       <c r="E15" s="108"/>
@@ -4907,7 +4909,7 @@
       <c r="C17" s="108"/>
       <c r="D17" s="108"/>
       <c r="E17" s="108" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F17" s="103" t="s">
         <v>5</v>
@@ -4916,18 +4918,18 @@
         <v>2013</v>
       </c>
       <c r="H17" s="104" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I17" s="104"/>
       <c r="J17" s="104"/>
       <c r="K17" s="116" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="2:11">
       <c r="B18" s="100"/>
       <c r="C18" s="112" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D18" s="108"/>
       <c r="E18" s="108"/>
@@ -4941,7 +4943,7 @@
     <row r="19" spans="2:11">
       <c r="B19" s="100"/>
       <c r="C19" s="112" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D19" s="108"/>
       <c r="E19" s="103"/>
@@ -4969,7 +4971,7 @@
       <c r="C21" s="108"/>
       <c r="D21" s="108"/>
       <c r="E21" s="95" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F21" s="108" t="s">
         <v>5</v>
@@ -4977,21 +4979,21 @@
       <c r="G21" s="108"/>
       <c r="H21" s="108"/>
       <c r="I21" s="108" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J21" s="119"/>
       <c r="K21" s="116" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22" spans="2:11">
       <c r="B22" s="100"/>
       <c r="C22" s="112" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D22" s="108"/>
       <c r="E22" s="103" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F22" s="108"/>
       <c r="G22" s="108"/>
@@ -5017,7 +5019,7 @@
       <c r="C24" s="108"/>
       <c r="D24" s="108"/>
       <c r="E24" s="103" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F24" s="108" t="s">
         <v>5</v>
@@ -5025,21 +5027,21 @@
       <c r="G24" s="108"/>
       <c r="H24" s="108"/>
       <c r="I24" s="108" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J24" s="119"/>
       <c r="K24" s="116" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" spans="2:11">
       <c r="B25" s="100"/>
       <c r="C25" s="112" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D25" s="108"/>
       <c r="E25" s="103" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F25" s="108"/>
       <c r="G25" s="108"/>
@@ -5105,7 +5107,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -5151,7 +5153,7 @@
     <row r="6" spans="2:14">
       <c r="B6" s="145"/>
       <c r="C6" s="146" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D6" s="146"/>
       <c r="E6" s="146"/>
@@ -5168,7 +5170,7 @@
     <row r="7" spans="2:14">
       <c r="B7" s="145"/>
       <c r="C7" s="146" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D7" s="146"/>
       <c r="E7" s="146"/>
@@ -5354,7 +5356,7 @@
         <v>2700</v>
       </c>
       <c r="E19" s="146" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F19" s="146"/>
       <c r="G19" s="146"/>
@@ -5373,7 +5375,7 @@
         <v>27</v>
       </c>
       <c r="E20" s="146" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F20" s="146"/>
       <c r="G20" s="146"/>
@@ -5392,7 +5394,7 @@
         <v>15</v>
       </c>
       <c r="E21" s="146" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F21" s="146"/>
       <c r="G21" s="146"/>
@@ -5437,7 +5439,7 @@
     <row r="24" spans="2:14">
       <c r="B24" s="145"/>
       <c r="C24" s="146" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D24" s="146"/>
       <c r="E24" s="146"/>
@@ -5638,7 +5640,7 @@
         <v>4800000</v>
       </c>
       <c r="E37" s="146" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F37" s="146"/>
       <c r="G37" s="146"/>
@@ -5713,7 +5715,7 @@
     <row r="42" spans="2:14">
       <c r="B42" s="145"/>
       <c r="C42" s="146" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D42" s="146"/>
       <c r="E42" s="146"/>
@@ -5730,7 +5732,7 @@
     <row r="43" spans="2:14">
       <c r="B43" s="145"/>
       <c r="C43" s="146" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D43" s="146"/>
       <c r="E43" s="146"/>
@@ -5797,7 +5799,7 @@
         <v>2.5</v>
       </c>
       <c r="F47" s="146" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G47" s="146"/>
       <c r="H47" s="146"/>
@@ -5891,7 +5893,7 @@
         <v>20</v>
       </c>
       <c r="F53" s="146" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G53" s="146"/>
       <c r="H53" s="146"/>
@@ -6010,7 +6012,7 @@
     <row r="61" spans="2:14">
       <c r="B61" s="145"/>
       <c r="C61" s="146" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D61" s="146"/>
       <c r="E61" s="146"/>
@@ -6027,7 +6029,7 @@
     <row r="62" spans="2:14">
       <c r="B62" s="145"/>
       <c r="C62" s="146" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D62" s="146"/>
       <c r="E62" s="146"/>
@@ -6154,7 +6156,7 @@
         <v>30</v>
       </c>
       <c r="F70" s="146" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G70" s="146"/>
       <c r="H70" s="146"/>

</xml_diff>

<commit_message>
Published state of ETDataset on April 20 2020
</commit_message>
<xml_diff>
--- a/nodes_source_analyses/energy/energy_chp_supercritical_waste_mix.central_producer.xlsx
+++ b/nodes_source_analyses/energy/energy_chp_supercritical_waste_mix.central_producer.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10113"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marliekeverweij/Projects/etdataset/nodes_source_analyses/energy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B523E6A-37D5-2349-90B5-2627D67D2D46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997FC87B-BE1E-B643-8537-8E18ADEE0782}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="28340" tabRatio="762" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,7 +48,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -59,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="153">
   <si>
     <t>Source</t>
   </si>
@@ -296,9 +298,6 @@
   </si>
   <si>
     <t>availability</t>
-  </si>
-  <si>
-    <t>capacity_credit</t>
   </si>
   <si>
     <t>forecasting_error</t>
@@ -437,21 +436,6 @@
     <t xml:space="preserve">        Fixed operating and maintenance costs </t>
   </si>
   <si>
-    <t>hours_prep_nl</t>
-  </si>
-  <si>
-    <t>hours_prod_nl</t>
-  </si>
-  <si>
-    <t>hours_place_nl</t>
-  </si>
-  <si>
-    <t>hours_maint_nl</t>
-  </si>
-  <si>
-    <t>hours_remov_nl</t>
-  </si>
-  <si>
     <t xml:space="preserve">         Land use per unit</t>
   </si>
   <si>
@@ -468,9 +452,6 @@
   </si>
   <si>
     <t>Heat output capacity</t>
-  </si>
-  <si>
-    <t>hours</t>
   </si>
   <si>
     <r>
@@ -825,6 +806,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -832,18 +814,21 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="16"/>
       <color theme="3"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -851,6 +836,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -858,17 +844,20 @@
       <sz val="12"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -952,7 +941,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -1183,17 +1172,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="263">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1460,7 +1438,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="157">
+  <cellXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -1643,10 +1621,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
@@ -1661,9 +1635,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
@@ -1680,6 +1652,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1707,7 +1680,6 @@
     <xf numFmtId="0" fontId="17" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="263">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2684,12 +2656,12 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="2.140625" style="50" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="50" customWidth="1"/>
+    <col min="1" max="1" width="2.1640625" style="50" customWidth="1"/>
+    <col min="2" max="2" width="9.5" style="50" customWidth="1"/>
     <col min="3" max="3" width="36" style="50" customWidth="1"/>
-    <col min="4" max="16384" width="10.7109375" style="50"/>
+    <col min="4" max="16384" width="10.6640625" style="50"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:3" s="48" customFormat="1"/>
@@ -2704,7 +2676,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="2:3" s="48" customFormat="1">
@@ -2825,57 +2797,57 @@
   <sheetPr codeName="Sheet2">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="B1:K43"/>
+  <dimension ref="B1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="2" width="2.42578125" style="17" customWidth="1"/>
-    <col min="3" max="3" width="45.42578125" style="17" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" style="17" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" style="17" customWidth="1"/>
-    <col min="6" max="6" width="2.140625" style="17" customWidth="1"/>
-    <col min="7" max="7" width="45.140625" style="17" customWidth="1"/>
-    <col min="8" max="8" width="2.140625" style="17" customWidth="1"/>
-    <col min="9" max="9" width="46.140625" style="17" customWidth="1"/>
-    <col min="10" max="10" width="2.140625" style="17" customWidth="1"/>
-    <col min="11" max="16384" width="10.7109375" style="17"/>
+    <col min="1" max="2" width="2.5" style="17" customWidth="1"/>
+    <col min="3" max="3" width="45.5" style="17" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" style="17" customWidth="1"/>
+    <col min="5" max="5" width="17.5" style="17" customWidth="1"/>
+    <col min="6" max="6" width="2.1640625" style="17" customWidth="1"/>
+    <col min="7" max="7" width="45.1640625" style="17" customWidth="1"/>
+    <col min="8" max="8" width="2.1640625" style="17" customWidth="1"/>
+    <col min="9" max="9" width="46.1640625" style="17" customWidth="1"/>
+    <col min="10" max="10" width="2.1640625" style="17" customWidth="1"/>
+    <col min="11" max="16384" width="10.6640625" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11">
       <c r="D1" s="14"/>
     </row>
     <row r="2" spans="2:11" ht="16" customHeight="1">
-      <c r="B2" s="147" t="s">
-        <v>158</v>
-      </c>
-      <c r="C2" s="148"/>
-      <c r="D2" s="148"/>
-      <c r="E2" s="149"/>
+      <c r="B2" s="142" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" s="143"/>
+      <c r="D2" s="143"/>
+      <c r="E2" s="144"/>
       <c r="F2" s="42"/>
     </row>
     <row r="3" spans="2:11">
-      <c r="B3" s="150"/>
-      <c r="C3" s="151"/>
-      <c r="D3" s="151"/>
-      <c r="E3" s="152"/>
+      <c r="B3" s="145"/>
+      <c r="C3" s="146"/>
+      <c r="D3" s="146"/>
+      <c r="E3" s="147"/>
       <c r="F3" s="42"/>
     </row>
     <row r="4" spans="2:11">
-      <c r="B4" s="150"/>
-      <c r="C4" s="151"/>
-      <c r="D4" s="151"/>
-      <c r="E4" s="152"/>
+      <c r="B4" s="145"/>
+      <c r="C4" s="146"/>
+      <c r="D4" s="146"/>
+      <c r="E4" s="147"/>
       <c r="F4" s="42"/>
     </row>
     <row r="5" spans="2:11">
-      <c r="B5" s="153"/>
-      <c r="C5" s="154"/>
-      <c r="D5" s="154"/>
-      <c r="E5" s="155"/>
+      <c r="B5" s="148"/>
+      <c r="C5" s="149"/>
+      <c r="D5" s="149"/>
+      <c r="E5" s="150"/>
       <c r="F5" s="42"/>
     </row>
     <row r="6" spans="2:11" ht="17" thickBot="1">
@@ -2963,7 +2935,7 @@
     <row r="12" spans="2:11" ht="17" thickBot="1">
       <c r="B12" s="21"/>
       <c r="C12" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>34</v>
@@ -2974,7 +2946,7 @@
       </c>
       <c r="F12" s="24"/>
       <c r="G12" s="63" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H12" s="24"/>
       <c r="I12" s="25" t="s">
@@ -3054,7 +3026,7 @@
         <v>2</v>
       </c>
       <c r="E16" s="68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" s="24"/>
       <c r="G16" s="63"/>
@@ -3088,13 +3060,13 @@
     <row r="18" spans="2:11" ht="17" thickBot="1">
       <c r="B18" s="21"/>
       <c r="C18" s="63" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E18" s="68">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F18" s="24"/>
       <c r="G18" s="63"/>
@@ -3105,7 +3077,7 @@
       <c r="J18" s="22"/>
       <c r="K18" s="14"/>
     </row>
-    <row r="19" spans="2:11" ht="17" thickBot="1">
+    <row r="19" spans="2:11">
       <c r="B19" s="21"/>
       <c r="C19" s="63" t="s">
         <v>83</v>
@@ -3114,7 +3086,7 @@
         <v>2</v>
       </c>
       <c r="E19" s="68">
-        <v>0.1</v>
+        <v>0.7</v>
       </c>
       <c r="F19" s="24"/>
       <c r="G19" s="63"/>
@@ -3127,69 +3099,71 @@
     </row>
     <row r="20" spans="2:11">
       <c r="B20" s="21"/>
-      <c r="C20" s="63" t="s">
-        <v>84</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E20" s="68">
-        <v>0.7</v>
-      </c>
-      <c r="F20" s="24"/>
-      <c r="G20" s="63"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="69" t="s">
-        <v>27</v>
-      </c>
+      <c r="C20" s="66"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
       <c r="J20" s="22"/>
       <c r="K20" s="14"/>
     </row>
-    <row r="21" spans="2:11">
+    <row r="21" spans="2:11" ht="17" thickBot="1">
       <c r="B21" s="21"/>
-      <c r="C21" s="66"/>
+      <c r="C21" s="11" t="s">
+        <v>31</v>
+      </c>
       <c r="D21" s="36"/>
-      <c r="E21" s="26"/>
+      <c r="E21" s="38"/>
       <c r="F21" s="14"/>
       <c r="G21" s="37"/>
       <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
+      <c r="I21" s="18"/>
       <c r="J21" s="22"/>
       <c r="K21" s="14"/>
     </row>
     <row r="22" spans="2:11" ht="17" thickBot="1">
       <c r="B22" s="21"/>
-      <c r="C22" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" s="36"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="37"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="18"/>
+      <c r="C22" s="63" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" s="40">
+        <f>'Research data'!F19</f>
+        <v>162000000</v>
+      </c>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="H22" s="24"/>
+      <c r="I22" s="85" t="s">
+        <v>87</v>
+      </c>
       <c r="J22" s="22"/>
       <c r="K22" s="14"/>
     </row>
     <row r="23" spans="2:11" ht="17" thickBot="1">
       <c r="B23" s="21"/>
       <c r="C23" s="63" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>61</v>
       </c>
       <c r="E23" s="40">
-        <f>'Research data'!F19</f>
-        <v>162000000</v>
+        <v>0</v>
       </c>
       <c r="F23" s="24"/>
-      <c r="G23" s="24" t="s">
-        <v>18</v>
+      <c r="G23" s="63" t="s">
+        <v>68</v>
       </c>
       <c r="H23" s="24"/>
-      <c r="I23" s="85" t="s">
-        <v>88</v>
+      <c r="I23" s="25" t="s">
+        <v>27</v>
       </c>
       <c r="J23" s="22"/>
       <c r="K23" s="14"/>
@@ -3197,17 +3171,17 @@
     <row r="24" spans="2:11" ht="17" thickBot="1">
       <c r="B24" s="21"/>
       <c r="C24" s="63" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E24" s="40">
+      <c r="E24" s="65">
         <v>0</v>
       </c>
       <c r="F24" s="24"/>
       <c r="G24" s="63" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H24" s="24"/>
       <c r="I24" s="25" t="s">
@@ -3219,7 +3193,7 @@
     <row r="25" spans="2:11" ht="17" thickBot="1">
       <c r="B25" s="21"/>
       <c r="C25" s="63" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>61</v>
@@ -3229,7 +3203,7 @@
       </c>
       <c r="F25" s="24"/>
       <c r="G25" s="63" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="H25" s="24"/>
       <c r="I25" s="25" t="s">
@@ -3241,21 +3215,22 @@
     <row r="26" spans="2:11" ht="17" thickBot="1">
       <c r="B26" s="21"/>
       <c r="C26" s="63" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E26" s="65">
-        <v>0</v>
+        <f>'Research data'!F22</f>
+        <v>4800000</v>
       </c>
       <c r="F26" s="24"/>
       <c r="G26" s="63" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H26" s="24"/>
       <c r="I26" s="25" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="J26" s="22"/>
       <c r="K26" s="14"/>
@@ -3263,22 +3238,21 @@
     <row r="27" spans="2:11" ht="17" thickBot="1">
       <c r="B27" s="21"/>
       <c r="C27" s="63" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="E27" s="65">
-        <f>'Research data'!F22</f>
-        <v>4800000</v>
+        <v>63</v>
+      </c>
+      <c r="E27" s="40">
+        <v>0</v>
       </c>
       <c r="F27" s="24"/>
       <c r="G27" s="63" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H27" s="24"/>
       <c r="I27" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J27" s="22"/>
       <c r="K27" s="14"/>
@@ -3286,7 +3260,7 @@
     <row r="28" spans="2:11" ht="17" thickBot="1">
       <c r="B28" s="21"/>
       <c r="C28" s="63" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>63</v>
@@ -3296,297 +3270,185 @@
       </c>
       <c r="F28" s="24"/>
       <c r="G28" s="63" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H28" s="24"/>
       <c r="I28" s="25" t="s">
-        <v>108</v>
+        <v>27</v>
       </c>
       <c r="J28" s="22"/>
       <c r="K28" s="14"/>
     </row>
     <row r="29" spans="2:11" ht="17" thickBot="1">
       <c r="B29" s="21"/>
-      <c r="C29" s="63" t="s">
-        <v>58</v>
+      <c r="C29" s="64" t="s">
+        <v>60</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="E29" s="40">
-        <v>0</v>
+        <v>115</v>
+      </c>
+      <c r="E29" s="67">
+        <v>0.04</v>
       </c>
       <c r="F29" s="24"/>
-      <c r="G29" s="63" t="s">
-        <v>67</v>
+      <c r="G29" s="24" t="s">
+        <v>71</v>
       </c>
       <c r="H29" s="24"/>
-      <c r="I29" s="25" t="s">
-        <v>27</v>
+      <c r="I29" s="141" t="s">
+        <v>152</v>
       </c>
       <c r="J29" s="22"/>
       <c r="K29" s="14"/>
     </row>
     <row r="30" spans="2:11" ht="17" thickBot="1">
       <c r="B30" s="21"/>
-      <c r="C30" s="64" t="s">
-        <v>60</v>
+      <c r="C30" s="63" t="s">
+        <v>81</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="E30" s="67">
-        <v>0.04</v>
+        <v>86</v>
+      </c>
+      <c r="E30" s="62">
+        <v>1</v>
       </c>
       <c r="F30" s="24"/>
-      <c r="G30" s="24" t="s">
-        <v>71</v>
-      </c>
+      <c r="G30" s="63"/>
       <c r="H30" s="24"/>
-      <c r="I30" s="156" t="s">
-        <v>159</v>
+      <c r="I30" s="140" t="s">
+        <v>27</v>
       </c>
       <c r="J30" s="22"/>
       <c r="K30" s="14"/>
     </row>
-    <row r="31" spans="2:11" ht="17" thickBot="1">
+    <row r="31" spans="2:11">
       <c r="B31" s="21"/>
-      <c r="C31" s="63" t="s">
-        <v>82</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="E31" s="62">
-        <v>1</v>
-      </c>
-      <c r="F31" s="24"/>
-      <c r="G31" s="63"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="146" t="s">
-        <v>27</v>
-      </c>
+      <c r="C31" s="35"/>
+      <c r="D31" s="36"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
       <c r="J31" s="22"/>
       <c r="K31" s="14"/>
     </row>
-    <row r="32" spans="2:11">
+    <row r="32" spans="2:11" ht="17" thickBot="1">
       <c r="B32" s="21"/>
-      <c r="C32" s="35"/>
+      <c r="C32" s="11" t="s">
+        <v>4</v>
+      </c>
       <c r="D32" s="36"/>
-      <c r="E32" s="27"/>
+      <c r="E32" s="39"/>
       <c r="F32" s="14"/>
       <c r="G32" s="14"/>
       <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
+      <c r="I32" s="18"/>
       <c r="J32" s="22"/>
       <c r="K32" s="14"/>
     </row>
     <row r="33" spans="2:11" ht="17" thickBot="1">
       <c r="B33" s="21"/>
-      <c r="C33" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" s="36"/>
-      <c r="E33" s="39"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="18"/>
+      <c r="C33" s="64" t="s">
+        <v>59</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E33" s="70">
+        <f>'Research data'!F13</f>
+        <v>3.5</v>
+      </c>
+      <c r="F33" s="24"/>
+      <c r="G33" s="63" t="s">
+        <v>70</v>
+      </c>
+      <c r="H33" s="24"/>
+      <c r="I33" s="85" t="s">
+        <v>27</v>
+      </c>
       <c r="J33" s="22"/>
       <c r="K33" s="14"/>
     </row>
     <row r="34" spans="2:11" ht="17" thickBot="1">
       <c r="B34" s="21"/>
       <c r="C34" s="64" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="D34" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E34" s="70">
-        <f>'Research data'!F13</f>
-        <v>3.5</v>
+      <c r="E34" s="86">
+        <f>'Research data'!F12</f>
+        <v>30</v>
       </c>
       <c r="F34" s="24"/>
-      <c r="G34" s="63" t="s">
-        <v>70</v>
+      <c r="G34" s="34" t="s">
+        <v>29</v>
       </c>
       <c r="H34" s="24"/>
       <c r="I34" s="85" t="s">
-        <v>27</v>
+        <v>143</v>
       </c>
       <c r="J34" s="22"/>
       <c r="K34" s="14"/>
     </row>
     <row r="35" spans="2:11" ht="17" thickBot="1">
       <c r="B35" s="21"/>
-      <c r="C35" s="64" t="s">
-        <v>23</v>
+      <c r="C35" s="28" t="s">
+        <v>73</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E35" s="86">
-        <f>'Research data'!F12</f>
-        <v>30</v>
+        <v>74</v>
+      </c>
+      <c r="E35" s="62">
+        <f>'Research data'!F14</f>
+        <v>0.1</v>
       </c>
       <c r="F35" s="24"/>
-      <c r="G35" s="34" t="s">
-        <v>29</v>
+      <c r="G35" s="63" t="s">
+        <v>75</v>
       </c>
       <c r="H35" s="24"/>
       <c r="I35" s="85" t="s">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="J35" s="22"/>
       <c r="K35" s="14"/>
     </row>
     <row r="36" spans="2:11" ht="17" thickBot="1">
       <c r="B36" s="21"/>
-      <c r="C36" s="28" t="s">
-        <v>73</v>
+      <c r="C36" s="33" t="s">
+        <v>28</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="E36" s="62">
-        <f>'Research data'!F14</f>
-        <v>0.1</v>
+        <v>2</v>
+      </c>
+      <c r="E36" s="41">
+        <v>0</v>
       </c>
       <c r="F36" s="24"/>
       <c r="G36" s="63" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H36" s="24"/>
-      <c r="I36" s="85" t="s">
-        <v>115</v>
+      <c r="I36" s="25" t="s">
+        <v>27</v>
       </c>
       <c r="J36" s="22"/>
       <c r="K36" s="14"/>
     </row>
     <row r="37" spans="2:11" ht="17" thickBot="1">
-      <c r="B37" s="21"/>
-      <c r="C37" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E37" s="41">
-        <v>0</v>
-      </c>
-      <c r="F37" s="24"/>
-      <c r="G37" s="63" t="s">
-        <v>72</v>
-      </c>
-      <c r="H37" s="24"/>
-      <c r="I37" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="J37" s="22"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="18"/>
+      <c r="J37" s="29"/>
       <c r="K37" s="14"/>
-    </row>
-    <row r="38" spans="2:11" ht="17" thickBot="1">
-      <c r="B38" s="21"/>
-      <c r="C38" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="D38" s="132" t="s">
-        <v>130</v>
-      </c>
-      <c r="E38" s="122"/>
-      <c r="F38" s="134"/>
-      <c r="G38" s="63"/>
-      <c r="H38" s="24"/>
-      <c r="I38" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="J38" s="22"/>
-      <c r="K38" s="14"/>
-    </row>
-    <row r="39" spans="2:11" ht="17" thickBot="1">
-      <c r="B39" s="21"/>
-      <c r="C39" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="D39" s="132" t="s">
-        <v>130</v>
-      </c>
-      <c r="E39" s="125"/>
-      <c r="F39" s="134"/>
-      <c r="G39" s="63"/>
-      <c r="H39" s="24"/>
-      <c r="I39" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="J39" s="22"/>
-      <c r="K39" s="14"/>
-    </row>
-    <row r="40" spans="2:11" ht="17" thickBot="1">
-      <c r="B40" s="21"/>
-      <c r="C40" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="D40" s="132" t="s">
-        <v>130</v>
-      </c>
-      <c r="E40" s="123"/>
-      <c r="F40" s="134"/>
-      <c r="G40" s="63"/>
-      <c r="H40" s="24"/>
-      <c r="I40" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="J40" s="22"/>
-      <c r="K40" s="14"/>
-    </row>
-    <row r="41" spans="2:11" ht="17" thickBot="1">
-      <c r="B41" s="21"/>
-      <c r="C41" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="D41" s="132" t="s">
-        <v>130</v>
-      </c>
-      <c r="E41" s="125"/>
-      <c r="F41" s="134"/>
-      <c r="G41" s="63"/>
-      <c r="H41" s="24"/>
-      <c r="I41" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="J41" s="22"/>
-      <c r="K41" s="14"/>
-    </row>
-    <row r="42" spans="2:11" ht="17" thickBot="1">
-      <c r="B42" s="21"/>
-      <c r="C42" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="D42" s="132" t="s">
-        <v>130</v>
-      </c>
-      <c r="E42" s="124"/>
-      <c r="F42" s="134"/>
-      <c r="G42" s="63"/>
-      <c r="H42" s="24"/>
-      <c r="I42" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="J42" s="22"/>
-      <c r="K42" s="14"/>
-    </row>
-    <row r="43" spans="2:11" ht="17" thickBot="1">
-      <c r="B43" s="23"/>
-      <c r="C43" s="30"/>
-      <c r="D43" s="31"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="18"/>
-      <c r="I43" s="18"/>
-      <c r="J43" s="29"/>
-      <c r="K43" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3608,26 +3470,26 @@
       <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="2" width="2.140625" style="79" customWidth="1"/>
-    <col min="3" max="3" width="37.140625" style="79" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" style="79" customWidth="1"/>
-    <col min="5" max="5" width="3.42578125" style="79" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" style="79" customWidth="1"/>
-    <col min="7" max="7" width="2.140625" style="79" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" style="79" customWidth="1"/>
-    <col min="9" max="9" width="2.140625" style="79" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" style="79" customWidth="1"/>
-    <col min="11" max="11" width="3.28515625" style="79" customWidth="1"/>
+    <col min="1" max="2" width="2.1640625" style="79" customWidth="1"/>
+    <col min="3" max="3" width="37.1640625" style="79" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="79" customWidth="1"/>
+    <col min="5" max="5" width="3.5" style="79" customWidth="1"/>
+    <col min="6" max="6" width="9.5" style="79" customWidth="1"/>
+    <col min="7" max="7" width="2.1640625" style="79" customWidth="1"/>
+    <col min="8" max="8" width="10.5" style="79" customWidth="1"/>
+    <col min="9" max="9" width="2.1640625" style="79" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" style="79" customWidth="1"/>
+    <col min="11" max="11" width="3.33203125" style="79" customWidth="1"/>
     <col min="12" max="12" width="9" style="79" customWidth="1"/>
-    <col min="13" max="13" width="2.140625" style="79" customWidth="1"/>
-    <col min="14" max="14" width="9.28515625" style="79" customWidth="1"/>
-    <col min="15" max="15" width="2.140625" style="79" customWidth="1"/>
-    <col min="16" max="16" width="7.42578125" style="79" customWidth="1"/>
-    <col min="17" max="17" width="2.140625" style="79" customWidth="1"/>
-    <col min="18" max="18" width="70.85546875" style="79" customWidth="1"/>
-    <col min="19" max="16384" width="10.7109375" style="79"/>
+    <col min="13" max="13" width="2.1640625" style="79" customWidth="1"/>
+    <col min="14" max="14" width="9.33203125" style="79" customWidth="1"/>
+    <col min="15" max="15" width="2.1640625" style="79" customWidth="1"/>
+    <col min="16" max="16" width="7.5" style="79" customWidth="1"/>
+    <col min="17" max="17" width="2.1640625" style="79" customWidth="1"/>
+    <col min="18" max="18" width="70.83203125" style="79" customWidth="1"/>
+    <col min="19" max="16384" width="10.6640625" style="79"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="17" thickBot="1"/>
@@ -3664,23 +3526,23 @@
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="K3" s="4"/>
       <c r="L3" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M3" s="4"/>
       <c r="N3" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O3" s="4"/>
       <c r="P3" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q3" s="4"/>
       <c r="R3" s="4" t="s">
@@ -3756,10 +3618,10 @@
     </row>
     <row r="7" spans="2:18" ht="17" thickBot="1">
       <c r="B7" s="73"/>
-      <c r="C7" s="131" t="s">
-        <v>129</v>
-      </c>
-      <c r="D7" s="126" t="s">
+      <c r="C7" s="127" t="s">
+        <v>123</v>
+      </c>
+      <c r="D7" s="122" t="s">
         <v>34</v>
       </c>
       <c r="E7" s="77"/>
@@ -3783,10 +3645,10 @@
     <row r="8" spans="2:18" ht="17" thickBot="1">
       <c r="B8" s="73"/>
       <c r="C8" s="121" t="s">
-        <v>127</v>
-      </c>
-      <c r="D8" s="126" t="s">
-        <v>116</v>
+        <v>121</v>
+      </c>
+      <c r="D8" s="122" t="s">
+        <v>115</v>
       </c>
       <c r="E8" s="77"/>
       <c r="F8" s="78">
@@ -3807,18 +3669,18 @@
       <c r="O8" s="88"/>
       <c r="P8" s="88"/>
       <c r="Q8" s="66"/>
-      <c r="R8" s="133"/>
+      <c r="R8" s="128"/>
     </row>
     <row r="9" spans="2:18" ht="17" thickBot="1">
       <c r="B9" s="73"/>
-      <c r="C9" s="129" t="s">
-        <v>128</v>
-      </c>
-      <c r="D9" s="130" t="s">
-        <v>116</v>
+      <c r="C9" s="125" t="s">
+        <v>122</v>
+      </c>
+      <c r="D9" s="126" t="s">
+        <v>115</v>
       </c>
       <c r="E9" s="66"/>
-      <c r="F9" s="127">
+      <c r="F9" s="123">
         <f>ROUND(15,1)</f>
         <v>15</v>
       </c>
@@ -3840,7 +3702,7 @@
     </row>
     <row r="10" spans="2:18">
       <c r="B10" s="73"/>
-      <c r="R10" s="133"/>
+      <c r="R10" s="128"/>
     </row>
     <row r="11" spans="2:18" ht="17" thickBot="1">
       <c r="B11" s="73"/>
@@ -3866,7 +3728,7 @@
     <row r="12" spans="2:18" ht="17" thickBot="1">
       <c r="B12" s="73"/>
       <c r="C12" s="121" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D12" s="76" t="s">
         <v>1</v>
@@ -3898,7 +3760,7 @@
     <row r="13" spans="2:18" ht="17" thickBot="1">
       <c r="B13" s="73"/>
       <c r="C13" s="121" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D13" s="76" t="s">
         <v>1</v>
@@ -3927,7 +3789,7 @@
     <row r="14" spans="2:18" ht="17" thickBot="1">
       <c r="B14" s="73"/>
       <c r="C14" s="121" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D14" s="76" t="s">
         <v>74</v>
@@ -3955,7 +3817,7 @@
       </c>
       <c r="Q14" s="66"/>
       <c r="R14" s="81" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="2:18">
@@ -3970,12 +3832,12 @@
       <c r="P15" s="88"/>
       <c r="Q15" s="66"/>
       <c r="R15" s="82" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="2:18">
       <c r="B16" s="73"/>
-      <c r="C16" s="128"/>
+      <c r="C16" s="124"/>
       <c r="D16" s="77"/>
       <c r="E16" s="77"/>
       <c r="F16" s="88"/>
@@ -3991,12 +3853,12 @@
       <c r="P16" s="88"/>
       <c r="Q16" s="66"/>
       <c r="R16" s="82" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="2:18">
       <c r="B17" s="73"/>
-      <c r="C17" s="128"/>
+      <c r="C17" s="124"/>
       <c r="D17" s="77"/>
       <c r="E17" s="77"/>
       <c r="F17" s="88"/>
@@ -4037,7 +3899,7 @@
     <row r="19" spans="2:18" ht="17" thickBot="1">
       <c r="B19" s="73"/>
       <c r="C19" s="75" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D19" s="75" t="s">
         <v>61</v>
@@ -4068,8 +3930,8 @@
       <c r="C20" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="135" t="s">
-        <v>132</v>
+      <c r="D20" s="129" t="s">
+        <v>125</v>
       </c>
       <c r="E20" s="11"/>
       <c r="F20" s="78">
@@ -4089,14 +3951,14 @@
       <c r="O20" s="83"/>
       <c r="P20" s="83"/>
       <c r="Q20" s="66"/>
-      <c r="R20" s="140" t="s">
-        <v>152</v>
+      <c r="R20" s="134" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="21" spans="2:18" ht="17" thickBot="1">
       <c r="B21" s="73"/>
-      <c r="C21" s="136" t="s">
-        <v>136</v>
+      <c r="C21" s="130" t="s">
+        <v>129</v>
       </c>
       <c r="D21" s="75" t="s">
         <v>61</v>
@@ -4125,7 +3987,7 @@
     <row r="22" spans="2:18" ht="17" thickBot="1">
       <c r="B22" s="73"/>
       <c r="C22" s="89" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D22" s="75" t="s">
         <v>62</v>
@@ -4146,17 +4008,17 @@
       <c r="O22" s="66"/>
       <c r="P22" s="66"/>
       <c r="Q22" s="66"/>
-      <c r="R22" s="138" t="s">
-        <v>131</v>
+      <c r="R22" s="132" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="2:18" ht="17" thickBot="1">
       <c r="B23" s="73"/>
       <c r="C23" s="89" t="s">
-        <v>118</v>
-      </c>
-      <c r="D23" s="136" t="s">
-        <v>133</v>
+        <v>117</v>
+      </c>
+      <c r="D23" s="130" t="s">
+        <v>126</v>
       </c>
       <c r="E23" s="90"/>
       <c r="F23" s="78">
@@ -4174,13 +4036,13 @@
       <c r="P23" s="66"/>
       <c r="Q23" s="66"/>
       <c r="R23" s="82" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="2:18" ht="17" thickBot="1">
       <c r="B24" s="73"/>
       <c r="C24" s="89" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D24" s="76" t="s">
         <v>63</v>
@@ -4205,7 +4067,7 @@
     <row r="25" spans="2:18" ht="17" thickBot="1">
       <c r="B25" s="73"/>
       <c r="C25" s="89" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="D25" s="76" t="s">
         <v>62</v>
@@ -4230,10 +4092,10 @@
     <row r="26" spans="2:18" ht="17" thickBot="1">
       <c r="B26" s="73"/>
       <c r="C26" s="89" t="s">
-        <v>99</v>
-      </c>
-      <c r="D26" s="135" t="s">
-        <v>134</v>
+        <v>98</v>
+      </c>
+      <c r="D26" s="129" t="s">
+        <v>127</v>
       </c>
       <c r="E26" s="91"/>
       <c r="F26" s="78">
@@ -4255,10 +4117,10 @@
     <row r="27" spans="2:18" ht="17" thickBot="1">
       <c r="B27" s="73"/>
       <c r="C27" s="92" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D27" s="63" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E27" s="91"/>
       <c r="F27" s="78">
@@ -4279,11 +4141,11 @@
     </row>
     <row r="28" spans="2:18" ht="17" thickBot="1">
       <c r="B28" s="73"/>
-      <c r="C28" s="138" t="s">
-        <v>138</v>
-      </c>
-      <c r="D28" s="137" t="s">
-        <v>135</v>
+      <c r="C28" s="132" t="s">
+        <v>131</v>
+      </c>
+      <c r="D28" s="131" t="s">
+        <v>128</v>
       </c>
       <c r="E28" s="91"/>
       <c r="F28" s="78">
@@ -4335,18 +4197,18 @@
       <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="33.140625" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="33.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="93" customWidth="1"/>
-    <col min="2" max="2" width="5.7109375" style="93" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" style="93" customWidth="1"/>
-    <col min="4" max="4" width="3.140625" style="93" customWidth="1"/>
-    <col min="5" max="5" width="26.7109375" style="93" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" style="93" customWidth="1"/>
-    <col min="7" max="9" width="12.140625" style="93" customWidth="1"/>
-    <col min="10" max="10" width="32.7109375" style="94" customWidth="1"/>
-    <col min="11" max="11" width="105.42578125" style="93" customWidth="1"/>
-    <col min="12" max="16384" width="33.140625" style="93"/>
+    <col min="1" max="1" width="10.1640625" style="93" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" style="93" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" style="93" customWidth="1"/>
+    <col min="4" max="4" width="3.1640625" style="93" customWidth="1"/>
+    <col min="5" max="5" width="26.6640625" style="93" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="93" customWidth="1"/>
+    <col min="7" max="9" width="12.1640625" style="93" customWidth="1"/>
+    <col min="10" max="10" width="32.6640625" style="94" customWidth="1"/>
+    <col min="11" max="11" width="105.5" style="93" customWidth="1"/>
+    <col min="12" max="16384" width="33.1640625" style="93"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="17" thickBot="1"/>
@@ -4404,13 +4266,13 @@
         <v>15</v>
       </c>
       <c r="H5" s="104" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="I5" s="104" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J5" s="105" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="K5" s="104" t="s">
         <v>8</v>
@@ -4433,10 +4295,10 @@
       <c r="C7" s="106"/>
       <c r="D7" s="106"/>
       <c r="E7" s="101" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="F7" s="101" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G7" s="102" t="s">
         <v>21</v>
@@ -4446,16 +4308,16 @@
       </c>
       <c r="I7" s="102"/>
       <c r="J7" s="102" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="K7" s="107" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="2:11">
       <c r="B8" s="98"/>
       <c r="C8" s="108" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D8" s="109"/>
       <c r="E8" s="101"/>
@@ -4483,7 +4345,7 @@
       <c r="C10" s="106"/>
       <c r="D10" s="106"/>
       <c r="E10" s="106" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F10" s="111" t="s">
         <v>22</v>
@@ -4492,20 +4354,20 @@
         <v>2000</v>
       </c>
       <c r="H10" s="112" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="I10" s="113"/>
       <c r="J10" s="112" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="K10" s="114" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="2:11">
       <c r="B11" s="98"/>
       <c r="C11" s="115" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D11" s="116"/>
       <c r="E11" s="106"/>
@@ -4533,20 +4395,20 @@
       <c r="C13" s="106"/>
       <c r="D13" s="106"/>
       <c r="E13" s="106" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F13" s="101" t="s">
         <v>5</v>
       </c>
       <c r="G13" s="102" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H13" s="102" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I13" s="102"/>
       <c r="J13" s="102" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="K13" s="114"/>
     </row>
@@ -4567,7 +4429,7 @@
     <row r="15" spans="2:11">
       <c r="B15" s="98"/>
       <c r="C15" s="110" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D15" s="106"/>
       <c r="E15" s="106"/>
@@ -4595,7 +4457,7 @@
       <c r="C17" s="106"/>
       <c r="D17" s="106"/>
       <c r="E17" s="106" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F17" s="101" t="s">
         <v>5</v>
@@ -4604,18 +4466,18 @@
         <v>2013</v>
       </c>
       <c r="H17" s="102" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="I17" s="102"/>
       <c r="J17" s="102"/>
       <c r="K17" s="114" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="2:11">
       <c r="B18" s="98"/>
       <c r="C18" s="110" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D18" s="106"/>
       <c r="E18" s="106"/>
@@ -4629,7 +4491,7 @@
     <row r="19" spans="2:11">
       <c r="B19" s="98"/>
       <c r="C19" s="110" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D19" s="106"/>
       <c r="E19" s="101"/>
@@ -4657,7 +4519,7 @@
       <c r="C21" s="106"/>
       <c r="D21" s="106"/>
       <c r="E21" s="93" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F21" s="106" t="s">
         <v>5</v>
@@ -4665,21 +4527,21 @@
       <c r="G21" s="106"/>
       <c r="H21" s="106"/>
       <c r="I21" s="106" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J21" s="117"/>
       <c r="K21" s="114" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="2:11">
       <c r="B22" s="98"/>
       <c r="C22" s="110" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D22" s="106"/>
       <c r="E22" s="101" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F22" s="106"/>
       <c r="G22" s="106"/>
@@ -4705,7 +4567,7 @@
       <c r="C24" s="106"/>
       <c r="D24" s="106"/>
       <c r="E24" s="101" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F24" s="106" t="s">
         <v>5</v>
@@ -4713,21 +4575,21 @@
       <c r="G24" s="106"/>
       <c r="H24" s="106"/>
       <c r="I24" s="106" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J24" s="117"/>
       <c r="K24" s="114" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="2:11">
       <c r="B25" s="98"/>
       <c r="C25" s="110" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D25" s="106"/>
       <c r="E25" s="101" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F25" s="106"/>
       <c r="G25" s="106"/>
@@ -4759,36 +4621,36 @@
       <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" style="139" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" style="139" customWidth="1"/>
-    <col min="3" max="16384" width="10.7109375" style="139"/>
+    <col min="1" max="1" width="6.33203125" style="133" customWidth="1"/>
+    <col min="2" max="2" width="5.5" style="133" customWidth="1"/>
+    <col min="3" max="16384" width="10.6640625" style="133"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="17" thickBot="1"/>
     <row r="2" spans="2:14">
-      <c r="B2" s="141"/>
-      <c r="C2" s="142"/>
-      <c r="D2" s="142"/>
-      <c r="E2" s="142"/>
-      <c r="F2" s="142"/>
-      <c r="G2" s="142"/>
-      <c r="H2" s="142"/>
-      <c r="I2" s="142"/>
-      <c r="J2" s="142"/>
-      <c r="K2" s="142"/>
-      <c r="L2" s="142"/>
-      <c r="M2" s="142"/>
-      <c r="N2" s="142"/>
+      <c r="B2" s="135"/>
+      <c r="C2" s="136"/>
+      <c r="D2" s="136"/>
+      <c r="E2" s="136"/>
+      <c r="F2" s="136"/>
+      <c r="G2" s="136"/>
+      <c r="H2" s="136"/>
+      <c r="I2" s="136"/>
+      <c r="J2" s="136"/>
+      <c r="K2" s="136"/>
+      <c r="L2" s="136"/>
+      <c r="M2" s="136"/>
+      <c r="N2" s="136"/>
     </row>
     <row r="3" spans="2:14" s="9" customFormat="1">
-      <c r="B3" s="145"/>
+      <c r="B3" s="139"/>
       <c r="C3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -4802,1186 +4664,1186 @@
       <c r="N3" s="4"/>
     </row>
     <row r="4" spans="2:14">
-      <c r="B4" s="143"/>
-      <c r="C4" s="144"/>
-      <c r="D4" s="144"/>
-      <c r="E4" s="144"/>
-      <c r="F4" s="144"/>
-      <c r="G4" s="144"/>
-      <c r="H4" s="144"/>
-      <c r="I4" s="144"/>
-      <c r="J4" s="144"/>
-      <c r="K4" s="144"/>
-      <c r="L4" s="144"/>
-      <c r="M4" s="144"/>
-      <c r="N4" s="144"/>
+      <c r="B4" s="137"/>
+      <c r="C4" s="138"/>
+      <c r="D4" s="138"/>
+      <c r="E4" s="138"/>
+      <c r="F4" s="138"/>
+      <c r="G4" s="138"/>
+      <c r="H4" s="138"/>
+      <c r="I4" s="138"/>
+      <c r="J4" s="138"/>
+      <c r="K4" s="138"/>
+      <c r="L4" s="138"/>
+      <c r="M4" s="138"/>
+      <c r="N4" s="138"/>
     </row>
     <row r="5" spans="2:14">
-      <c r="B5" s="143"/>
-      <c r="C5" s="144"/>
-      <c r="D5" s="144"/>
-      <c r="E5" s="144"/>
-      <c r="F5" s="144"/>
-      <c r="G5" s="144"/>
-      <c r="H5" s="144"/>
-      <c r="I5" s="144"/>
-      <c r="J5" s="144"/>
-      <c r="K5" s="144"/>
-      <c r="L5" s="144"/>
-      <c r="M5" s="144"/>
-      <c r="N5" s="144"/>
+      <c r="B5" s="137"/>
+      <c r="C5" s="138"/>
+      <c r="D5" s="138"/>
+      <c r="E5" s="138"/>
+      <c r="F5" s="138"/>
+      <c r="G5" s="138"/>
+      <c r="H5" s="138"/>
+      <c r="I5" s="138"/>
+      <c r="J5" s="138"/>
+      <c r="K5" s="138"/>
+      <c r="L5" s="138"/>
+      <c r="M5" s="138"/>
+      <c r="N5" s="138"/>
     </row>
     <row r="6" spans="2:14">
-      <c r="B6" s="143"/>
-      <c r="C6" s="144" t="s">
-        <v>88</v>
-      </c>
-      <c r="D6" s="144"/>
-      <c r="E6" s="144"/>
-      <c r="F6" s="144"/>
-      <c r="G6" s="144"/>
-      <c r="H6" s="144"/>
-      <c r="I6" s="144"/>
-      <c r="J6" s="144"/>
-      <c r="K6" s="144"/>
-      <c r="L6" s="144"/>
-      <c r="M6" s="144"/>
-      <c r="N6" s="144"/>
+      <c r="B6" s="137"/>
+      <c r="C6" s="138" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" s="138"/>
+      <c r="E6" s="138"/>
+      <c r="F6" s="138"/>
+      <c r="G6" s="138"/>
+      <c r="H6" s="138"/>
+      <c r="I6" s="138"/>
+      <c r="J6" s="138"/>
+      <c r="K6" s="138"/>
+      <c r="L6" s="138"/>
+      <c r="M6" s="138"/>
+      <c r="N6" s="138"/>
     </row>
     <row r="7" spans="2:14">
-      <c r="B7" s="143"/>
-      <c r="C7" s="144" t="s">
+      <c r="B7" s="137"/>
+      <c r="C7" s="138" t="s">
+        <v>134</v>
+      </c>
+      <c r="D7" s="138"/>
+      <c r="E7" s="138"/>
+      <c r="F7" s="138"/>
+      <c r="G7" s="138"/>
+      <c r="H7" s="138"/>
+      <c r="I7" s="138"/>
+      <c r="J7" s="138"/>
+      <c r="K7" s="138"/>
+      <c r="L7" s="138"/>
+      <c r="M7" s="138"/>
+      <c r="N7" s="138"/>
+    </row>
+    <row r="8" spans="2:14">
+      <c r="B8" s="137"/>
+      <c r="C8" s="138"/>
+      <c r="D8" s="138"/>
+      <c r="E8" s="138"/>
+      <c r="F8" s="138"/>
+      <c r="G8" s="138"/>
+      <c r="H8" s="138"/>
+      <c r="I8" s="138"/>
+      <c r="J8" s="138"/>
+      <c r="K8" s="138"/>
+      <c r="L8" s="138"/>
+      <c r="M8" s="138"/>
+      <c r="N8" s="138"/>
+    </row>
+    <row r="9" spans="2:14">
+      <c r="B9" s="137"/>
+      <c r="C9" s="138"/>
+      <c r="D9" s="138"/>
+      <c r="E9" s="138"/>
+      <c r="F9" s="138"/>
+      <c r="G9" s="138"/>
+      <c r="H9" s="138"/>
+      <c r="I9" s="138"/>
+      <c r="J9" s="138"/>
+      <c r="K9" s="138"/>
+      <c r="L9" s="138"/>
+      <c r="M9" s="138"/>
+      <c r="N9" s="138"/>
+    </row>
+    <row r="10" spans="2:14">
+      <c r="B10" s="137"/>
+      <c r="C10" s="138"/>
+      <c r="D10" s="138"/>
+      <c r="E10" s="138"/>
+      <c r="F10" s="138"/>
+      <c r="G10" s="138"/>
+      <c r="H10" s="138"/>
+      <c r="I10" s="138"/>
+      <c r="J10" s="138"/>
+      <c r="K10" s="138"/>
+      <c r="L10" s="138"/>
+      <c r="M10" s="138"/>
+      <c r="N10" s="138"/>
+    </row>
+    <row r="11" spans="2:14">
+      <c r="B11" s="137"/>
+      <c r="C11" s="138"/>
+      <c r="D11" s="138"/>
+      <c r="E11" s="138"/>
+      <c r="F11" s="138"/>
+      <c r="G11" s="138"/>
+      <c r="H11" s="138"/>
+      <c r="I11" s="138"/>
+      <c r="J11" s="138"/>
+      <c r="K11" s="138"/>
+      <c r="L11" s="138"/>
+      <c r="M11" s="138"/>
+      <c r="N11" s="138"/>
+    </row>
+    <row r="12" spans="2:14">
+      <c r="B12" s="137"/>
+      <c r="C12" s="138"/>
+      <c r="D12" s="138"/>
+      <c r="E12" s="138"/>
+      <c r="F12" s="138"/>
+      <c r="G12" s="138"/>
+      <c r="H12" s="138"/>
+      <c r="I12" s="138"/>
+      <c r="J12" s="138"/>
+      <c r="K12" s="138"/>
+      <c r="L12" s="138"/>
+      <c r="M12" s="138"/>
+      <c r="N12" s="138"/>
+    </row>
+    <row r="13" spans="2:14">
+      <c r="B13" s="137"/>
+      <c r="C13" s="138"/>
+      <c r="D13" s="138"/>
+      <c r="E13" s="138"/>
+      <c r="F13" s="138"/>
+      <c r="G13" s="138"/>
+      <c r="H13" s="138"/>
+      <c r="I13" s="138"/>
+      <c r="J13" s="138"/>
+      <c r="K13" s="138"/>
+      <c r="L13" s="138"/>
+      <c r="M13" s="138"/>
+      <c r="N13" s="138"/>
+    </row>
+    <row r="14" spans="2:14">
+      <c r="B14" s="137"/>
+      <c r="C14" s="138"/>
+      <c r="D14" s="138"/>
+      <c r="E14" s="138"/>
+      <c r="F14" s="138"/>
+      <c r="G14" s="138"/>
+      <c r="H14" s="138"/>
+      <c r="I14" s="138"/>
+      <c r="J14" s="138"/>
+      <c r="K14" s="138"/>
+      <c r="L14" s="138"/>
+      <c r="M14" s="138"/>
+      <c r="N14" s="138"/>
+    </row>
+    <row r="15" spans="2:14">
+      <c r="B15" s="137"/>
+      <c r="C15" s="138"/>
+      <c r="D15" s="138"/>
+      <c r="E15" s="138"/>
+      <c r="F15" s="138"/>
+      <c r="G15" s="138"/>
+      <c r="H15" s="138"/>
+      <c r="I15" s="138"/>
+      <c r="J15" s="138"/>
+      <c r="K15" s="138"/>
+      <c r="L15" s="138"/>
+      <c r="M15" s="138"/>
+      <c r="N15" s="138"/>
+    </row>
+    <row r="16" spans="2:14">
+      <c r="B16" s="137"/>
+      <c r="C16" s="138"/>
+      <c r="D16" s="138"/>
+      <c r="E16" s="138"/>
+      <c r="F16" s="138"/>
+      <c r="G16" s="138"/>
+      <c r="H16" s="138"/>
+      <c r="I16" s="138"/>
+      <c r="J16" s="138"/>
+      <c r="K16" s="138"/>
+      <c r="L16" s="138"/>
+      <c r="M16" s="138"/>
+      <c r="N16" s="138"/>
+    </row>
+    <row r="17" spans="2:14">
+      <c r="B17" s="137"/>
+      <c r="C17" s="138"/>
+      <c r="D17" s="138"/>
+      <c r="E17" s="138"/>
+      <c r="F17" s="138"/>
+      <c r="G17" s="138"/>
+      <c r="H17" s="138"/>
+      <c r="I17" s="138"/>
+      <c r="J17" s="138"/>
+      <c r="K17" s="138"/>
+      <c r="L17" s="138"/>
+      <c r="M17" s="138"/>
+      <c r="N17" s="138"/>
+    </row>
+    <row r="18" spans="2:14">
+      <c r="B18" s="137"/>
+      <c r="C18" s="138"/>
+      <c r="D18" s="138"/>
+      <c r="E18" s="138"/>
+      <c r="F18" s="138"/>
+      <c r="G18" s="138"/>
+      <c r="H18" s="138"/>
+      <c r="I18" s="138"/>
+      <c r="J18" s="138"/>
+      <c r="K18" s="138"/>
+      <c r="L18" s="138"/>
+      <c r="M18" s="138"/>
+      <c r="N18" s="138"/>
+    </row>
+    <row r="19" spans="2:14">
+      <c r="B19" s="137"/>
+      <c r="C19" s="138"/>
+      <c r="D19" s="138">
+        <v>2700</v>
+      </c>
+      <c r="E19" s="138" t="s">
+        <v>136</v>
+      </c>
+      <c r="F19" s="138"/>
+      <c r="G19" s="138"/>
+      <c r="H19" s="138"/>
+      <c r="I19" s="138"/>
+      <c r="J19" s="138"/>
+      <c r="K19" s="138"/>
+      <c r="L19" s="138"/>
+      <c r="M19" s="138"/>
+      <c r="N19" s="138"/>
+    </row>
+    <row r="20" spans="2:14">
+      <c r="B20" s="137"/>
+      <c r="C20" s="138"/>
+      <c r="D20" s="138">
+        <v>27</v>
+      </c>
+      <c r="E20" s="138" t="s">
+        <v>115</v>
+      </c>
+      <c r="F20" s="138"/>
+      <c r="G20" s="138"/>
+      <c r="H20" s="138"/>
+      <c r="I20" s="138"/>
+      <c r="J20" s="138"/>
+      <c r="K20" s="138"/>
+      <c r="L20" s="138"/>
+      <c r="M20" s="138"/>
+      <c r="N20" s="138"/>
+    </row>
+    <row r="21" spans="2:14">
+      <c r="B21" s="137"/>
+      <c r="C21" s="138"/>
+      <c r="D21" s="138">
+        <v>15</v>
+      </c>
+      <c r="E21" s="138" t="s">
+        <v>115</v>
+      </c>
+      <c r="F21" s="138"/>
+      <c r="G21" s="138"/>
+      <c r="H21" s="138"/>
+      <c r="I21" s="138"/>
+      <c r="J21" s="138"/>
+      <c r="K21" s="138"/>
+      <c r="L21" s="138"/>
+      <c r="M21" s="138"/>
+      <c r="N21" s="138"/>
+    </row>
+    <row r="22" spans="2:14">
+      <c r="B22" s="137"/>
+      <c r="C22" s="138"/>
+      <c r="D22" s="138"/>
+      <c r="E22" s="138"/>
+      <c r="F22" s="138"/>
+      <c r="G22" s="138"/>
+      <c r="H22" s="138"/>
+      <c r="I22" s="138"/>
+      <c r="J22" s="138"/>
+      <c r="K22" s="138"/>
+      <c r="L22" s="138"/>
+      <c r="M22" s="138"/>
+      <c r="N22" s="138"/>
+    </row>
+    <row r="23" spans="2:14">
+      <c r="B23" s="137"/>
+      <c r="C23" s="138"/>
+      <c r="D23" s="138"/>
+      <c r="E23" s="138"/>
+      <c r="F23" s="138"/>
+      <c r="G23" s="138"/>
+      <c r="H23" s="138"/>
+      <c r="I23" s="138"/>
+      <c r="J23" s="138"/>
+      <c r="K23" s="138"/>
+      <c r="L23" s="138"/>
+      <c r="M23" s="138"/>
+      <c r="N23" s="138"/>
+    </row>
+    <row r="24" spans="2:14">
+      <c r="B24" s="137"/>
+      <c r="C24" s="138" t="s">
+        <v>135</v>
+      </c>
+      <c r="D24" s="138"/>
+      <c r="E24" s="138"/>
+      <c r="F24" s="138"/>
+      <c r="G24" s="138"/>
+      <c r="H24" s="138"/>
+      <c r="I24" s="138"/>
+      <c r="J24" s="138"/>
+      <c r="K24" s="138"/>
+      <c r="L24" s="138"/>
+      <c r="M24" s="138"/>
+      <c r="N24" s="138"/>
+    </row>
+    <row r="25" spans="2:14">
+      <c r="B25" s="137"/>
+      <c r="C25" s="138"/>
+      <c r="D25" s="138"/>
+      <c r="E25" s="138"/>
+      <c r="F25" s="138"/>
+      <c r="G25" s="138"/>
+      <c r="H25" s="138"/>
+      <c r="I25" s="138"/>
+      <c r="J25" s="138"/>
+      <c r="K25" s="138"/>
+      <c r="L25" s="138"/>
+      <c r="M25" s="138"/>
+      <c r="N25" s="138"/>
+    </row>
+    <row r="26" spans="2:14">
+      <c r="B26" s="137"/>
+      <c r="C26" s="138"/>
+      <c r="D26" s="138"/>
+      <c r="E26" s="138"/>
+      <c r="F26" s="138"/>
+      <c r="G26" s="138"/>
+      <c r="H26" s="138"/>
+      <c r="I26" s="138"/>
+      <c r="J26" s="138"/>
+      <c r="K26" s="138"/>
+      <c r="L26" s="138"/>
+      <c r="M26" s="138"/>
+      <c r="N26" s="138"/>
+    </row>
+    <row r="27" spans="2:14">
+      <c r="B27" s="137"/>
+      <c r="C27" s="138"/>
+      <c r="D27" s="138"/>
+      <c r="E27" s="138"/>
+      <c r="F27" s="138"/>
+      <c r="G27" s="138"/>
+      <c r="H27" s="138"/>
+      <c r="I27" s="138"/>
+      <c r="J27" s="138"/>
+      <c r="K27" s="138"/>
+      <c r="L27" s="138"/>
+      <c r="M27" s="138"/>
+      <c r="N27" s="138"/>
+    </row>
+    <row r="28" spans="2:14">
+      <c r="B28" s="137"/>
+      <c r="C28" s="138"/>
+      <c r="D28" s="138"/>
+      <c r="E28" s="138"/>
+      <c r="F28" s="138"/>
+      <c r="G28" s="138"/>
+      <c r="H28" s="138"/>
+      <c r="I28" s="138"/>
+      <c r="J28" s="138"/>
+      <c r="K28" s="138"/>
+      <c r="L28" s="138"/>
+      <c r="M28" s="138"/>
+      <c r="N28" s="138"/>
+    </row>
+    <row r="29" spans="2:14">
+      <c r="B29" s="137"/>
+      <c r="C29" s="138"/>
+      <c r="D29" s="138"/>
+      <c r="E29" s="138"/>
+      <c r="F29" s="138"/>
+      <c r="G29" s="138"/>
+      <c r="H29" s="138"/>
+      <c r="I29" s="138"/>
+      <c r="J29" s="138"/>
+      <c r="K29" s="138"/>
+      <c r="L29" s="138"/>
+      <c r="M29" s="138"/>
+      <c r="N29" s="138"/>
+    </row>
+    <row r="30" spans="2:14">
+      <c r="B30" s="137"/>
+      <c r="C30" s="138"/>
+      <c r="D30" s="138"/>
+      <c r="E30" s="138"/>
+      <c r="F30" s="138"/>
+      <c r="G30" s="138"/>
+      <c r="H30" s="138"/>
+      <c r="I30" s="138"/>
+      <c r="J30" s="138"/>
+      <c r="K30" s="138"/>
+      <c r="L30" s="138"/>
+      <c r="M30" s="138"/>
+      <c r="N30" s="138"/>
+    </row>
+    <row r="31" spans="2:14">
+      <c r="B31" s="137"/>
+      <c r="C31" s="138"/>
+      <c r="D31" s="138"/>
+      <c r="E31" s="138"/>
+      <c r="F31" s="138"/>
+      <c r="G31" s="138"/>
+      <c r="H31" s="138"/>
+      <c r="I31" s="138"/>
+      <c r="J31" s="138"/>
+      <c r="K31" s="138"/>
+      <c r="L31" s="138"/>
+      <c r="M31" s="138"/>
+      <c r="N31" s="138"/>
+    </row>
+    <row r="32" spans="2:14">
+      <c r="B32" s="137"/>
+      <c r="C32" s="138"/>
+      <c r="D32" s="138"/>
+      <c r="E32" s="138"/>
+      <c r="F32" s="138"/>
+      <c r="G32" s="138"/>
+      <c r="H32" s="138"/>
+      <c r="I32" s="138"/>
+      <c r="J32" s="138"/>
+      <c r="K32" s="138"/>
+      <c r="L32" s="138"/>
+      <c r="M32" s="138"/>
+      <c r="N32" s="138"/>
+    </row>
+    <row r="33" spans="2:14">
+      <c r="B33" s="137"/>
+      <c r="C33" s="138"/>
+      <c r="D33" s="138"/>
+      <c r="E33" s="138"/>
+      <c r="F33" s="138"/>
+      <c r="G33" s="138"/>
+      <c r="H33" s="138"/>
+      <c r="I33" s="138"/>
+      <c r="J33" s="138"/>
+      <c r="K33" s="138"/>
+      <c r="L33" s="138"/>
+      <c r="M33" s="138"/>
+      <c r="N33" s="138"/>
+    </row>
+    <row r="34" spans="2:14">
+      <c r="B34" s="137"/>
+      <c r="C34" s="138"/>
+      <c r="D34" s="138"/>
+      <c r="E34" s="138"/>
+      <c r="F34" s="138"/>
+      <c r="G34" s="138"/>
+      <c r="H34" s="138"/>
+      <c r="I34" s="138"/>
+      <c r="J34" s="138"/>
+      <c r="K34" s="138"/>
+      <c r="L34" s="138"/>
+      <c r="M34" s="138"/>
+      <c r="N34" s="138"/>
+    </row>
+    <row r="35" spans="2:14">
+      <c r="B35" s="137"/>
+      <c r="C35" s="138"/>
+      <c r="D35" s="138"/>
+      <c r="E35" s="138"/>
+      <c r="F35" s="138"/>
+      <c r="G35" s="138"/>
+      <c r="H35" s="138"/>
+      <c r="I35" s="138"/>
+      <c r="J35" s="138"/>
+      <c r="K35" s="138"/>
+      <c r="L35" s="138"/>
+      <c r="M35" s="138"/>
+      <c r="N35" s="138"/>
+    </row>
+    <row r="36" spans="2:14">
+      <c r="B36" s="137"/>
+      <c r="C36" s="138"/>
+      <c r="D36" s="138"/>
+      <c r="E36" s="138"/>
+      <c r="F36" s="138"/>
+      <c r="G36" s="138"/>
+      <c r="H36" s="138"/>
+      <c r="I36" s="138"/>
+      <c r="J36" s="138"/>
+      <c r="K36" s="138"/>
+      <c r="L36" s="138"/>
+      <c r="M36" s="138"/>
+      <c r="N36" s="138"/>
+    </row>
+    <row r="37" spans="2:14">
+      <c r="B37" s="137"/>
+      <c r="C37" s="138"/>
+      <c r="D37" s="138">
+        <v>4800000</v>
+      </c>
+      <c r="E37" s="138" t="s">
+        <v>61</v>
+      </c>
+      <c r="F37" s="138"/>
+      <c r="G37" s="138"/>
+      <c r="H37" s="138"/>
+      <c r="I37" s="138"/>
+      <c r="J37" s="138"/>
+      <c r="K37" s="138"/>
+      <c r="L37" s="138"/>
+      <c r="M37" s="138"/>
+      <c r="N37" s="138"/>
+    </row>
+    <row r="38" spans="2:14">
+      <c r="B38" s="137"/>
+      <c r="C38" s="138"/>
+      <c r="D38" s="138"/>
+      <c r="E38" s="138"/>
+      <c r="F38" s="138"/>
+      <c r="G38" s="138"/>
+      <c r="H38" s="138"/>
+      <c r="I38" s="138"/>
+      <c r="J38" s="138"/>
+      <c r="K38" s="138"/>
+      <c r="L38" s="138"/>
+      <c r="M38" s="138"/>
+      <c r="N38" s="138"/>
+    </row>
+    <row r="39" spans="2:14">
+      <c r="B39" s="137"/>
+      <c r="C39" s="138"/>
+      <c r="D39" s="138"/>
+      <c r="E39" s="138"/>
+      <c r="F39" s="138"/>
+      <c r="G39" s="138"/>
+      <c r="H39" s="138"/>
+      <c r="I39" s="138"/>
+      <c r="J39" s="138"/>
+      <c r="K39" s="138"/>
+      <c r="L39" s="138"/>
+      <c r="M39" s="138"/>
+      <c r="N39" s="138"/>
+    </row>
+    <row r="40" spans="2:14">
+      <c r="B40" s="137"/>
+      <c r="C40" s="138"/>
+      <c r="D40" s="138"/>
+      <c r="E40" s="138"/>
+      <c r="F40" s="138"/>
+      <c r="G40" s="138"/>
+      <c r="H40" s="138"/>
+      <c r="I40" s="138"/>
+      <c r="J40" s="138"/>
+      <c r="K40" s="138"/>
+      <c r="L40" s="138"/>
+      <c r="M40" s="138"/>
+      <c r="N40" s="138"/>
+    </row>
+    <row r="41" spans="2:14">
+      <c r="B41" s="137"/>
+      <c r="C41" s="138"/>
+      <c r="D41" s="138"/>
+      <c r="E41" s="138"/>
+      <c r="F41" s="138"/>
+      <c r="G41" s="138"/>
+      <c r="H41" s="138"/>
+      <c r="I41" s="138"/>
+      <c r="J41" s="138"/>
+      <c r="K41" s="138"/>
+      <c r="L41" s="138"/>
+      <c r="M41" s="138"/>
+      <c r="N41" s="138"/>
+    </row>
+    <row r="42" spans="2:14">
+      <c r="B42" s="137"/>
+      <c r="C42" s="138" t="s">
+        <v>138</v>
+      </c>
+      <c r="D42" s="138"/>
+      <c r="E42" s="138"/>
+      <c r="F42" s="138"/>
+      <c r="G42" s="138"/>
+      <c r="H42" s="138"/>
+      <c r="I42" s="138"/>
+      <c r="J42" s="138"/>
+      <c r="K42" s="138"/>
+      <c r="L42" s="138"/>
+      <c r="M42" s="138"/>
+      <c r="N42" s="138"/>
+    </row>
+    <row r="43" spans="2:14">
+      <c r="B43" s="137"/>
+      <c r="C43" s="138" t="s">
+        <v>139</v>
+      </c>
+      <c r="D43" s="138"/>
+      <c r="E43" s="138"/>
+      <c r="F43" s="138"/>
+      <c r="G43" s="138"/>
+      <c r="H43" s="138"/>
+      <c r="I43" s="138"/>
+      <c r="J43" s="138"/>
+      <c r="K43" s="138"/>
+      <c r="L43" s="138"/>
+      <c r="M43" s="138"/>
+      <c r="N43" s="138"/>
+    </row>
+    <row r="44" spans="2:14">
+      <c r="B44" s="137"/>
+      <c r="C44" s="138"/>
+      <c r="D44" s="138"/>
+      <c r="E44" s="138"/>
+      <c r="F44" s="138"/>
+      <c r="G44" s="138"/>
+      <c r="H44" s="138"/>
+      <c r="I44" s="138"/>
+      <c r="J44" s="138"/>
+      <c r="K44" s="138"/>
+      <c r="L44" s="138"/>
+      <c r="M44" s="138"/>
+      <c r="N44" s="138"/>
+    </row>
+    <row r="45" spans="2:14">
+      <c r="B45" s="137"/>
+      <c r="C45" s="138"/>
+      <c r="D45" s="138"/>
+      <c r="E45" s="138"/>
+      <c r="F45" s="138"/>
+      <c r="G45" s="138"/>
+      <c r="H45" s="138"/>
+      <c r="I45" s="138"/>
+      <c r="J45" s="138"/>
+      <c r="K45" s="138"/>
+      <c r="L45" s="138"/>
+      <c r="M45" s="138"/>
+      <c r="N45" s="138"/>
+    </row>
+    <row r="46" spans="2:14">
+      <c r="B46" s="137"/>
+      <c r="C46" s="138"/>
+      <c r="D46" s="138"/>
+      <c r="E46" s="138"/>
+      <c r="F46" s="138"/>
+      <c r="G46" s="138"/>
+      <c r="H46" s="138"/>
+      <c r="I46" s="138"/>
+      <c r="J46" s="138"/>
+      <c r="K46" s="138"/>
+      <c r="L46" s="138"/>
+      <c r="M46" s="138"/>
+      <c r="N46" s="138"/>
+    </row>
+    <row r="47" spans="2:14">
+      <c r="B47" s="137"/>
+      <c r="C47" s="138"/>
+      <c r="D47" s="138"/>
+      <c r="E47" s="138">
+        <v>2.5</v>
+      </c>
+      <c r="F47" s="138" t="s">
+        <v>142</v>
+      </c>
+      <c r="G47" s="138"/>
+      <c r="H47" s="138"/>
+      <c r="I47" s="138"/>
+      <c r="J47" s="138"/>
+      <c r="K47" s="138"/>
+      <c r="L47" s="138"/>
+      <c r="M47" s="138"/>
+      <c r="N47" s="138"/>
+    </row>
+    <row r="48" spans="2:14">
+      <c r="B48" s="137"/>
+      <c r="C48" s="138"/>
+      <c r="D48" s="138"/>
+      <c r="E48" s="138"/>
+      <c r="F48" s="138"/>
+      <c r="G48" s="138"/>
+      <c r="H48" s="138"/>
+      <c r="I48" s="138"/>
+      <c r="J48" s="138"/>
+      <c r="K48" s="138"/>
+      <c r="L48" s="138"/>
+      <c r="M48" s="138"/>
+      <c r="N48" s="138"/>
+    </row>
+    <row r="49" spans="2:14">
+      <c r="B49" s="137"/>
+      <c r="C49" s="138"/>
+      <c r="D49" s="138"/>
+      <c r="E49" s="138"/>
+      <c r="F49" s="138"/>
+      <c r="G49" s="138"/>
+      <c r="H49" s="138"/>
+      <c r="I49" s="138"/>
+      <c r="J49" s="138"/>
+      <c r="K49" s="138"/>
+      <c r="L49" s="138"/>
+      <c r="M49" s="138"/>
+      <c r="N49" s="138"/>
+    </row>
+    <row r="50" spans="2:14">
+      <c r="B50" s="137"/>
+      <c r="C50" s="138"/>
+      <c r="D50" s="138"/>
+      <c r="E50" s="138"/>
+      <c r="F50" s="138"/>
+      <c r="G50" s="138"/>
+      <c r="H50" s="138"/>
+      <c r="I50" s="138"/>
+      <c r="J50" s="138"/>
+      <c r="K50" s="138"/>
+      <c r="L50" s="138"/>
+      <c r="M50" s="138"/>
+      <c r="N50" s="138"/>
+    </row>
+    <row r="51" spans="2:14">
+      <c r="B51" s="137"/>
+      <c r="C51" s="138"/>
+      <c r="D51" s="138"/>
+      <c r="E51" s="138"/>
+      <c r="F51" s="138"/>
+      <c r="G51" s="138"/>
+      <c r="H51" s="138"/>
+      <c r="I51" s="138"/>
+      <c r="J51" s="138"/>
+      <c r="K51" s="138"/>
+      <c r="L51" s="138"/>
+      <c r="M51" s="138"/>
+      <c r="N51" s="138"/>
+    </row>
+    <row r="52" spans="2:14">
+      <c r="B52" s="137"/>
+      <c r="C52" s="138"/>
+      <c r="D52" s="138"/>
+      <c r="E52" s="138"/>
+      <c r="F52" s="138"/>
+      <c r="G52" s="138"/>
+      <c r="H52" s="138"/>
+      <c r="I52" s="138"/>
+      <c r="J52" s="138"/>
+      <c r="K52" s="138"/>
+      <c r="L52" s="138"/>
+      <c r="M52" s="138"/>
+      <c r="N52" s="138"/>
+    </row>
+    <row r="53" spans="2:14">
+      <c r="B53" s="137"/>
+      <c r="C53" s="138"/>
+      <c r="D53" s="138"/>
+      <c r="E53" s="138">
+        <v>20</v>
+      </c>
+      <c r="F53" s="138" t="s">
+        <v>142</v>
+      </c>
+      <c r="G53" s="138"/>
+      <c r="H53" s="138"/>
+      <c r="I53" s="138"/>
+      <c r="J53" s="138"/>
+      <c r="K53" s="138"/>
+      <c r="L53" s="138"/>
+      <c r="M53" s="138"/>
+      <c r="N53" s="138"/>
+    </row>
+    <row r="54" spans="2:14">
+      <c r="B54" s="137"/>
+      <c r="C54" s="138"/>
+      <c r="D54" s="138"/>
+      <c r="E54" s="138"/>
+      <c r="F54" s="138"/>
+      <c r="G54" s="138"/>
+      <c r="H54" s="138"/>
+      <c r="I54" s="138"/>
+      <c r="J54" s="138"/>
+      <c r="K54" s="138"/>
+      <c r="L54" s="138"/>
+      <c r="M54" s="138"/>
+      <c r="N54" s="138"/>
+    </row>
+    <row r="55" spans="2:14">
+      <c r="B55" s="137"/>
+      <c r="C55" s="138"/>
+      <c r="D55" s="138"/>
+      <c r="E55" s="138"/>
+      <c r="F55" s="138"/>
+      <c r="G55" s="138"/>
+      <c r="H55" s="138"/>
+      <c r="I55" s="138"/>
+      <c r="J55" s="138"/>
+      <c r="K55" s="138"/>
+      <c r="L55" s="138"/>
+      <c r="M55" s="138"/>
+      <c r="N55" s="138"/>
+    </row>
+    <row r="56" spans="2:14">
+      <c r="B56" s="137"/>
+      <c r="C56" s="138"/>
+      <c r="D56" s="138"/>
+      <c r="E56" s="138"/>
+      <c r="F56" s="138"/>
+      <c r="G56" s="138"/>
+      <c r="H56" s="138"/>
+      <c r="I56" s="138"/>
+      <c r="J56" s="138"/>
+      <c r="K56" s="138"/>
+      <c r="L56" s="138"/>
+      <c r="M56" s="138"/>
+      <c r="N56" s="138"/>
+    </row>
+    <row r="57" spans="2:14">
+      <c r="B57" s="137"/>
+      <c r="C57" s="138"/>
+      <c r="D57" s="138"/>
+      <c r="E57" s="138"/>
+      <c r="F57" s="138"/>
+      <c r="G57" s="138"/>
+      <c r="H57" s="138"/>
+      <c r="I57" s="138"/>
+      <c r="J57" s="138"/>
+      <c r="K57" s="138"/>
+      <c r="L57" s="138"/>
+      <c r="M57" s="138"/>
+      <c r="N57" s="138"/>
+    </row>
+    <row r="58" spans="2:14">
+      <c r="B58" s="137"/>
+      <c r="C58" s="138"/>
+      <c r="D58" s="138"/>
+      <c r="E58" s="138"/>
+      <c r="F58" s="138"/>
+      <c r="G58" s="138"/>
+      <c r="H58" s="138"/>
+      <c r="I58" s="138"/>
+      <c r="J58" s="138"/>
+      <c r="K58" s="138"/>
+      <c r="L58" s="138"/>
+      <c r="M58" s="138"/>
+      <c r="N58" s="138"/>
+    </row>
+    <row r="59" spans="2:14">
+      <c r="B59" s="137"/>
+      <c r="C59" s="138"/>
+      <c r="D59" s="138"/>
+      <c r="E59" s="138"/>
+      <c r="F59" s="138"/>
+      <c r="G59" s="138"/>
+      <c r="H59" s="138"/>
+      <c r="I59" s="138"/>
+      <c r="J59" s="138"/>
+      <c r="K59" s="138"/>
+      <c r="L59" s="138"/>
+      <c r="M59" s="138"/>
+      <c r="N59" s="138"/>
+    </row>
+    <row r="60" spans="2:14">
+      <c r="B60" s="137"/>
+      <c r="C60" s="138"/>
+      <c r="D60" s="138"/>
+      <c r="E60" s="138"/>
+      <c r="F60" s="138"/>
+      <c r="G60" s="138"/>
+      <c r="H60" s="138"/>
+      <c r="I60" s="138"/>
+      <c r="J60" s="138"/>
+      <c r="K60" s="138"/>
+      <c r="L60" s="138"/>
+      <c r="M60" s="138"/>
+      <c r="N60" s="138"/>
+    </row>
+    <row r="61" spans="2:14">
+      <c r="B61" s="137"/>
+      <c r="C61" s="138" t="s">
+        <v>140</v>
+      </c>
+      <c r="D61" s="138"/>
+      <c r="E61" s="138"/>
+      <c r="F61" s="138"/>
+      <c r="G61" s="138"/>
+      <c r="H61" s="138"/>
+      <c r="I61" s="138"/>
+      <c r="J61" s="138"/>
+      <c r="K61" s="138"/>
+      <c r="L61" s="138"/>
+      <c r="M61" s="138"/>
+      <c r="N61" s="138"/>
+    </row>
+    <row r="62" spans="2:14">
+      <c r="B62" s="137"/>
+      <c r="C62" s="138" t="s">
         <v>141</v>
       </c>
-      <c r="D7" s="144"/>
-      <c r="E7" s="144"/>
-      <c r="F7" s="144"/>
-      <c r="G7" s="144"/>
-      <c r="H7" s="144"/>
-      <c r="I7" s="144"/>
-      <c r="J7" s="144"/>
-      <c r="K7" s="144"/>
-      <c r="L7" s="144"/>
-      <c r="M7" s="144"/>
-      <c r="N7" s="144"/>
-    </row>
-    <row r="8" spans="2:14">
-      <c r="B8" s="143"/>
-      <c r="C8" s="144"/>
-      <c r="D8" s="144"/>
-      <c r="E8" s="144"/>
-      <c r="F8" s="144"/>
-      <c r="G8" s="144"/>
-      <c r="H8" s="144"/>
-      <c r="I8" s="144"/>
-      <c r="J8" s="144"/>
-      <c r="K8" s="144"/>
-      <c r="L8" s="144"/>
-      <c r="M8" s="144"/>
-      <c r="N8" s="144"/>
-    </row>
-    <row r="9" spans="2:14">
-      <c r="B9" s="143"/>
-      <c r="C9" s="144"/>
-      <c r="D9" s="144"/>
-      <c r="E9" s="144"/>
-      <c r="F9" s="144"/>
-      <c r="G9" s="144"/>
-      <c r="H9" s="144"/>
-      <c r="I9" s="144"/>
-      <c r="J9" s="144"/>
-      <c r="K9" s="144"/>
-      <c r="L9" s="144"/>
-      <c r="M9" s="144"/>
-      <c r="N9" s="144"/>
-    </row>
-    <row r="10" spans="2:14">
-      <c r="B10" s="143"/>
-      <c r="C10" s="144"/>
-      <c r="D10" s="144"/>
-      <c r="E10" s="144"/>
-      <c r="F10" s="144"/>
-      <c r="G10" s="144"/>
-      <c r="H10" s="144"/>
-      <c r="I10" s="144"/>
-      <c r="J10" s="144"/>
-      <c r="K10" s="144"/>
-      <c r="L10" s="144"/>
-      <c r="M10" s="144"/>
-      <c r="N10" s="144"/>
-    </row>
-    <row r="11" spans="2:14">
-      <c r="B11" s="143"/>
-      <c r="C11" s="144"/>
-      <c r="D11" s="144"/>
-      <c r="E11" s="144"/>
-      <c r="F11" s="144"/>
-      <c r="G11" s="144"/>
-      <c r="H11" s="144"/>
-      <c r="I11" s="144"/>
-      <c r="J11" s="144"/>
-      <c r="K11" s="144"/>
-      <c r="L11" s="144"/>
-      <c r="M11" s="144"/>
-      <c r="N11" s="144"/>
-    </row>
-    <row r="12" spans="2:14">
-      <c r="B12" s="143"/>
-      <c r="C12" s="144"/>
-      <c r="D12" s="144"/>
-      <c r="E12" s="144"/>
-      <c r="F12" s="144"/>
-      <c r="G12" s="144"/>
-      <c r="H12" s="144"/>
-      <c r="I12" s="144"/>
-      <c r="J12" s="144"/>
-      <c r="K12" s="144"/>
-      <c r="L12" s="144"/>
-      <c r="M12" s="144"/>
-      <c r="N12" s="144"/>
-    </row>
-    <row r="13" spans="2:14">
-      <c r="B13" s="143"/>
-      <c r="C13" s="144"/>
-      <c r="D13" s="144"/>
-      <c r="E13" s="144"/>
-      <c r="F13" s="144"/>
-      <c r="G13" s="144"/>
-      <c r="H13" s="144"/>
-      <c r="I13" s="144"/>
-      <c r="J13" s="144"/>
-      <c r="K13" s="144"/>
-      <c r="L13" s="144"/>
-      <c r="M13" s="144"/>
-      <c r="N13" s="144"/>
-    </row>
-    <row r="14" spans="2:14">
-      <c r="B14" s="143"/>
-      <c r="C14" s="144"/>
-      <c r="D14" s="144"/>
-      <c r="E14" s="144"/>
-      <c r="F14" s="144"/>
-      <c r="G14" s="144"/>
-      <c r="H14" s="144"/>
-      <c r="I14" s="144"/>
-      <c r="J14" s="144"/>
-      <c r="K14" s="144"/>
-      <c r="L14" s="144"/>
-      <c r="M14" s="144"/>
-      <c r="N14" s="144"/>
-    </row>
-    <row r="15" spans="2:14">
-      <c r="B15" s="143"/>
-      <c r="C15" s="144"/>
-      <c r="D15" s="144"/>
-      <c r="E15" s="144"/>
-      <c r="F15" s="144"/>
-      <c r="G15" s="144"/>
-      <c r="H15" s="144"/>
-      <c r="I15" s="144"/>
-      <c r="J15" s="144"/>
-      <c r="K15" s="144"/>
-      <c r="L15" s="144"/>
-      <c r="M15" s="144"/>
-      <c r="N15" s="144"/>
-    </row>
-    <row r="16" spans="2:14">
-      <c r="B16" s="143"/>
-      <c r="C16" s="144"/>
-      <c r="D16" s="144"/>
-      <c r="E16" s="144"/>
-      <c r="F16" s="144"/>
-      <c r="G16" s="144"/>
-      <c r="H16" s="144"/>
-      <c r="I16" s="144"/>
-      <c r="J16" s="144"/>
-      <c r="K16" s="144"/>
-      <c r="L16" s="144"/>
-      <c r="M16" s="144"/>
-      <c r="N16" s="144"/>
-    </row>
-    <row r="17" spans="2:14">
-      <c r="B17" s="143"/>
-      <c r="C17" s="144"/>
-      <c r="D17" s="144"/>
-      <c r="E17" s="144"/>
-      <c r="F17" s="144"/>
-      <c r="G17" s="144"/>
-      <c r="H17" s="144"/>
-      <c r="I17" s="144"/>
-      <c r="J17" s="144"/>
-      <c r="K17" s="144"/>
-      <c r="L17" s="144"/>
-      <c r="M17" s="144"/>
-      <c r="N17" s="144"/>
-    </row>
-    <row r="18" spans="2:14">
-      <c r="B18" s="143"/>
-      <c r="C18" s="144"/>
-      <c r="D18" s="144"/>
-      <c r="E18" s="144"/>
-      <c r="F18" s="144"/>
-      <c r="G18" s="144"/>
-      <c r="H18" s="144"/>
-      <c r="I18" s="144"/>
-      <c r="J18" s="144"/>
-      <c r="K18" s="144"/>
-      <c r="L18" s="144"/>
-      <c r="M18" s="144"/>
-      <c r="N18" s="144"/>
-    </row>
-    <row r="19" spans="2:14">
-      <c r="B19" s="143"/>
-      <c r="C19" s="144"/>
-      <c r="D19" s="144">
-        <v>2700</v>
-      </c>
-      <c r="E19" s="144" t="s">
-        <v>143</v>
-      </c>
-      <c r="F19" s="144"/>
-      <c r="G19" s="144"/>
-      <c r="H19" s="144"/>
-      <c r="I19" s="144"/>
-      <c r="J19" s="144"/>
-      <c r="K19" s="144"/>
-      <c r="L19" s="144"/>
-      <c r="M19" s="144"/>
-      <c r="N19" s="144"/>
-    </row>
-    <row r="20" spans="2:14">
-      <c r="B20" s="143"/>
-      <c r="C20" s="144"/>
-      <c r="D20" s="144">
-        <v>27</v>
-      </c>
-      <c r="E20" s="144" t="s">
-        <v>116</v>
-      </c>
-      <c r="F20" s="144"/>
-      <c r="G20" s="144"/>
-      <c r="H20" s="144"/>
-      <c r="I20" s="144"/>
-      <c r="J20" s="144"/>
-      <c r="K20" s="144"/>
-      <c r="L20" s="144"/>
-      <c r="M20" s="144"/>
-      <c r="N20" s="144"/>
-    </row>
-    <row r="21" spans="2:14">
-      <c r="B21" s="143"/>
-      <c r="C21" s="144"/>
-      <c r="D21" s="144">
-        <v>15</v>
-      </c>
-      <c r="E21" s="144" t="s">
-        <v>116</v>
-      </c>
-      <c r="F21" s="144"/>
-      <c r="G21" s="144"/>
-      <c r="H21" s="144"/>
-      <c r="I21" s="144"/>
-      <c r="J21" s="144"/>
-      <c r="K21" s="144"/>
-      <c r="L21" s="144"/>
-      <c r="M21" s="144"/>
-      <c r="N21" s="144"/>
-    </row>
-    <row r="22" spans="2:14">
-      <c r="B22" s="143"/>
-      <c r="C22" s="144"/>
-      <c r="D22" s="144"/>
-      <c r="E22" s="144"/>
-      <c r="F22" s="144"/>
-      <c r="G22" s="144"/>
-      <c r="H22" s="144"/>
-      <c r="I22" s="144"/>
-      <c r="J22" s="144"/>
-      <c r="K22" s="144"/>
-      <c r="L22" s="144"/>
-      <c r="M22" s="144"/>
-      <c r="N22" s="144"/>
-    </row>
-    <row r="23" spans="2:14">
-      <c r="B23" s="143"/>
-      <c r="C23" s="144"/>
-      <c r="D23" s="144"/>
-      <c r="E23" s="144"/>
-      <c r="F23" s="144"/>
-      <c r="G23" s="144"/>
-      <c r="H23" s="144"/>
-      <c r="I23" s="144"/>
-      <c r="J23" s="144"/>
-      <c r="K23" s="144"/>
-      <c r="L23" s="144"/>
-      <c r="M23" s="144"/>
-      <c r="N23" s="144"/>
-    </row>
-    <row r="24" spans="2:14">
-      <c r="B24" s="143"/>
-      <c r="C24" s="144" t="s">
+      <c r="D62" s="138"/>
+      <c r="E62" s="138"/>
+      <c r="F62" s="138"/>
+      <c r="G62" s="138"/>
+      <c r="H62" s="138"/>
+      <c r="I62" s="138"/>
+      <c r="J62" s="138"/>
+      <c r="K62" s="138"/>
+      <c r="L62" s="138"/>
+      <c r="M62" s="138"/>
+      <c r="N62" s="138"/>
+    </row>
+    <row r="63" spans="2:14">
+      <c r="B63" s="137"/>
+      <c r="C63" s="138"/>
+      <c r="D63" s="138"/>
+      <c r="E63" s="138"/>
+      <c r="F63" s="138"/>
+      <c r="G63" s="138"/>
+      <c r="H63" s="138"/>
+      <c r="I63" s="138"/>
+      <c r="J63" s="138"/>
+      <c r="K63" s="138"/>
+      <c r="L63" s="138"/>
+      <c r="M63" s="138"/>
+      <c r="N63" s="138"/>
+    </row>
+    <row r="64" spans="2:14">
+      <c r="B64" s="137"/>
+      <c r="C64" s="138"/>
+      <c r="D64" s="138"/>
+      <c r="E64" s="138"/>
+      <c r="F64" s="138"/>
+      <c r="G64" s="138"/>
+      <c r="H64" s="138"/>
+      <c r="I64" s="138"/>
+      <c r="J64" s="138"/>
+      <c r="K64" s="138"/>
+      <c r="L64" s="138"/>
+      <c r="M64" s="138"/>
+      <c r="N64" s="138"/>
+    </row>
+    <row r="65" spans="2:14">
+      <c r="B65" s="137"/>
+      <c r="C65" s="138"/>
+      <c r="D65" s="138"/>
+      <c r="E65" s="138"/>
+      <c r="F65" s="138"/>
+      <c r="G65" s="138"/>
+      <c r="H65" s="138"/>
+      <c r="I65" s="138"/>
+      <c r="J65" s="138"/>
+      <c r="K65" s="138"/>
+      <c r="L65" s="138"/>
+      <c r="M65" s="138"/>
+      <c r="N65" s="138"/>
+    </row>
+    <row r="66" spans="2:14">
+      <c r="B66" s="137"/>
+      <c r="C66" s="138"/>
+      <c r="D66" s="138"/>
+      <c r="E66" s="138"/>
+      <c r="F66" s="138"/>
+      <c r="G66" s="138"/>
+      <c r="H66" s="138"/>
+      <c r="I66" s="138"/>
+      <c r="J66" s="138"/>
+      <c r="K66" s="138"/>
+      <c r="L66" s="138"/>
+      <c r="M66" s="138"/>
+      <c r="N66" s="138"/>
+    </row>
+    <row r="67" spans="2:14">
+      <c r="B67" s="137"/>
+      <c r="C67" s="138"/>
+      <c r="D67" s="138"/>
+      <c r="E67" s="138"/>
+      <c r="F67" s="138"/>
+      <c r="G67" s="138"/>
+      <c r="H67" s="138"/>
+      <c r="I67" s="138"/>
+      <c r="J67" s="138"/>
+      <c r="K67" s="138"/>
+      <c r="L67" s="138"/>
+      <c r="M67" s="138"/>
+      <c r="N67" s="138"/>
+    </row>
+    <row r="68" spans="2:14">
+      <c r="B68" s="137"/>
+      <c r="C68" s="138"/>
+      <c r="D68" s="138"/>
+      <c r="E68" s="138"/>
+      <c r="F68" s="138"/>
+      <c r="G68" s="138"/>
+      <c r="H68" s="138"/>
+      <c r="I68" s="138"/>
+      <c r="J68" s="138"/>
+      <c r="K68" s="138"/>
+      <c r="L68" s="138"/>
+      <c r="M68" s="138"/>
+      <c r="N68" s="138"/>
+    </row>
+    <row r="69" spans="2:14">
+      <c r="B69" s="137"/>
+      <c r="C69" s="138"/>
+      <c r="D69" s="138"/>
+      <c r="E69" s="138"/>
+      <c r="F69" s="138"/>
+      <c r="G69" s="138"/>
+      <c r="H69" s="138"/>
+      <c r="I69" s="138"/>
+      <c r="J69" s="138"/>
+      <c r="K69" s="138"/>
+      <c r="L69" s="138"/>
+      <c r="M69" s="138"/>
+      <c r="N69" s="138"/>
+    </row>
+    <row r="70" spans="2:14">
+      <c r="B70" s="137"/>
+      <c r="C70" s="138"/>
+      <c r="D70" s="138"/>
+      <c r="E70" s="138">
+        <v>30</v>
+      </c>
+      <c r="F70" s="138" t="s">
         <v>142</v>
       </c>
-      <c r="D24" s="144"/>
-      <c r="E24" s="144"/>
-      <c r="F24" s="144"/>
-      <c r="G24" s="144"/>
-      <c r="H24" s="144"/>
-      <c r="I24" s="144"/>
-      <c r="J24" s="144"/>
-      <c r="K24" s="144"/>
-      <c r="L24" s="144"/>
-      <c r="M24" s="144"/>
-      <c r="N24" s="144"/>
-    </row>
-    <row r="25" spans="2:14">
-      <c r="B25" s="143"/>
-      <c r="C25" s="144"/>
-      <c r="D25" s="144"/>
-      <c r="E25" s="144"/>
-      <c r="F25" s="144"/>
-      <c r="G25" s="144"/>
-      <c r="H25" s="144"/>
-      <c r="I25" s="144"/>
-      <c r="J25" s="144"/>
-      <c r="K25" s="144"/>
-      <c r="L25" s="144"/>
-      <c r="M25" s="144"/>
-      <c r="N25" s="144"/>
-    </row>
-    <row r="26" spans="2:14">
-      <c r="B26" s="143"/>
-      <c r="C26" s="144"/>
-      <c r="D26" s="144"/>
-      <c r="E26" s="144"/>
-      <c r="F26" s="144"/>
-      <c r="G26" s="144"/>
-      <c r="H26" s="144"/>
-      <c r="I26" s="144"/>
-      <c r="J26" s="144"/>
-      <c r="K26" s="144"/>
-      <c r="L26" s="144"/>
-      <c r="M26" s="144"/>
-      <c r="N26" s="144"/>
-    </row>
-    <row r="27" spans="2:14">
-      <c r="B27" s="143"/>
-      <c r="C27" s="144"/>
-      <c r="D27" s="144"/>
-      <c r="E27" s="144"/>
-      <c r="F27" s="144"/>
-      <c r="G27" s="144"/>
-      <c r="H27" s="144"/>
-      <c r="I27" s="144"/>
-      <c r="J27" s="144"/>
-      <c r="K27" s="144"/>
-      <c r="L27" s="144"/>
-      <c r="M27" s="144"/>
-      <c r="N27" s="144"/>
-    </row>
-    <row r="28" spans="2:14">
-      <c r="B28" s="143"/>
-      <c r="C28" s="144"/>
-      <c r="D28" s="144"/>
-      <c r="E28" s="144"/>
-      <c r="F28" s="144"/>
-      <c r="G28" s="144"/>
-      <c r="H28" s="144"/>
-      <c r="I28" s="144"/>
-      <c r="J28" s="144"/>
-      <c r="K28" s="144"/>
-      <c r="L28" s="144"/>
-      <c r="M28" s="144"/>
-      <c r="N28" s="144"/>
-    </row>
-    <row r="29" spans="2:14">
-      <c r="B29" s="143"/>
-      <c r="C29" s="144"/>
-      <c r="D29" s="144"/>
-      <c r="E29" s="144"/>
-      <c r="F29" s="144"/>
-      <c r="G29" s="144"/>
-      <c r="H29" s="144"/>
-      <c r="I29" s="144"/>
-      <c r="J29" s="144"/>
-      <c r="K29" s="144"/>
-      <c r="L29" s="144"/>
-      <c r="M29" s="144"/>
-      <c r="N29" s="144"/>
-    </row>
-    <row r="30" spans="2:14">
-      <c r="B30" s="143"/>
-      <c r="C30" s="144"/>
-      <c r="D30" s="144"/>
-      <c r="E30" s="144"/>
-      <c r="F30" s="144"/>
-      <c r="G30" s="144"/>
-      <c r="H30" s="144"/>
-      <c r="I30" s="144"/>
-      <c r="J30" s="144"/>
-      <c r="K30" s="144"/>
-      <c r="L30" s="144"/>
-      <c r="M30" s="144"/>
-      <c r="N30" s="144"/>
-    </row>
-    <row r="31" spans="2:14">
-      <c r="B31" s="143"/>
-      <c r="C31" s="144"/>
-      <c r="D31" s="144"/>
-      <c r="E31" s="144"/>
-      <c r="F31" s="144"/>
-      <c r="G31" s="144"/>
-      <c r="H31" s="144"/>
-      <c r="I31" s="144"/>
-      <c r="J31" s="144"/>
-      <c r="K31" s="144"/>
-      <c r="L31" s="144"/>
-      <c r="M31" s="144"/>
-      <c r="N31" s="144"/>
-    </row>
-    <row r="32" spans="2:14">
-      <c r="B32" s="143"/>
-      <c r="C32" s="144"/>
-      <c r="D32" s="144"/>
-      <c r="E32" s="144"/>
-      <c r="F32" s="144"/>
-      <c r="G32" s="144"/>
-      <c r="H32" s="144"/>
-      <c r="I32" s="144"/>
-      <c r="J32" s="144"/>
-      <c r="K32" s="144"/>
-      <c r="L32" s="144"/>
-      <c r="M32" s="144"/>
-      <c r="N32" s="144"/>
-    </row>
-    <row r="33" spans="2:14">
-      <c r="B33" s="143"/>
-      <c r="C33" s="144"/>
-      <c r="D33" s="144"/>
-      <c r="E33" s="144"/>
-      <c r="F33" s="144"/>
-      <c r="G33" s="144"/>
-      <c r="H33" s="144"/>
-      <c r="I33" s="144"/>
-      <c r="J33" s="144"/>
-      <c r="K33" s="144"/>
-      <c r="L33" s="144"/>
-      <c r="M33" s="144"/>
-      <c r="N33" s="144"/>
-    </row>
-    <row r="34" spans="2:14">
-      <c r="B34" s="143"/>
-      <c r="C34" s="144"/>
-      <c r="D34" s="144"/>
-      <c r="E34" s="144"/>
-      <c r="F34" s="144"/>
-      <c r="G34" s="144"/>
-      <c r="H34" s="144"/>
-      <c r="I34" s="144"/>
-      <c r="J34" s="144"/>
-      <c r="K34" s="144"/>
-      <c r="L34" s="144"/>
-      <c r="M34" s="144"/>
-      <c r="N34" s="144"/>
-    </row>
-    <row r="35" spans="2:14">
-      <c r="B35" s="143"/>
-      <c r="C35" s="144"/>
-      <c r="D35" s="144"/>
-      <c r="E35" s="144"/>
-      <c r="F35" s="144"/>
-      <c r="G35" s="144"/>
-      <c r="H35" s="144"/>
-      <c r="I35" s="144"/>
-      <c r="J35" s="144"/>
-      <c r="K35" s="144"/>
-      <c r="L35" s="144"/>
-      <c r="M35" s="144"/>
-      <c r="N35" s="144"/>
-    </row>
-    <row r="36" spans="2:14">
-      <c r="B36" s="143"/>
-      <c r="C36" s="144"/>
-      <c r="D36" s="144"/>
-      <c r="E36" s="144"/>
-      <c r="F36" s="144"/>
-      <c r="G36" s="144"/>
-      <c r="H36" s="144"/>
-      <c r="I36" s="144"/>
-      <c r="J36" s="144"/>
-      <c r="K36" s="144"/>
-      <c r="L36" s="144"/>
-      <c r="M36" s="144"/>
-      <c r="N36" s="144"/>
-    </row>
-    <row r="37" spans="2:14">
-      <c r="B37" s="143"/>
-      <c r="C37" s="144"/>
-      <c r="D37" s="144">
-        <v>4800000</v>
-      </c>
-      <c r="E37" s="144" t="s">
-        <v>61</v>
-      </c>
-      <c r="F37" s="144"/>
-      <c r="G37" s="144"/>
-      <c r="H37" s="144"/>
-      <c r="I37" s="144"/>
-      <c r="J37" s="144"/>
-      <c r="K37" s="144"/>
-      <c r="L37" s="144"/>
-      <c r="M37" s="144"/>
-      <c r="N37" s="144"/>
-    </row>
-    <row r="38" spans="2:14">
-      <c r="B38" s="143"/>
-      <c r="C38" s="144"/>
-      <c r="D38" s="144"/>
-      <c r="E38" s="144"/>
-      <c r="F38" s="144"/>
-      <c r="G38" s="144"/>
-      <c r="H38" s="144"/>
-      <c r="I38" s="144"/>
-      <c r="J38" s="144"/>
-      <c r="K38" s="144"/>
-      <c r="L38" s="144"/>
-      <c r="M38" s="144"/>
-      <c r="N38" s="144"/>
-    </row>
-    <row r="39" spans="2:14">
-      <c r="B39" s="143"/>
-      <c r="C39" s="144"/>
-      <c r="D39" s="144"/>
-      <c r="E39" s="144"/>
-      <c r="F39" s="144"/>
-      <c r="G39" s="144"/>
-      <c r="H39" s="144"/>
-      <c r="I39" s="144"/>
-      <c r="J39" s="144"/>
-      <c r="K39" s="144"/>
-      <c r="L39" s="144"/>
-      <c r="M39" s="144"/>
-      <c r="N39" s="144"/>
-    </row>
-    <row r="40" spans="2:14">
-      <c r="B40" s="143"/>
-      <c r="C40" s="144"/>
-      <c r="D40" s="144"/>
-      <c r="E40" s="144"/>
-      <c r="F40" s="144"/>
-      <c r="G40" s="144"/>
-      <c r="H40" s="144"/>
-      <c r="I40" s="144"/>
-      <c r="J40" s="144"/>
-      <c r="K40" s="144"/>
-      <c r="L40" s="144"/>
-      <c r="M40" s="144"/>
-      <c r="N40" s="144"/>
-    </row>
-    <row r="41" spans="2:14">
-      <c r="B41" s="143"/>
-      <c r="C41" s="144"/>
-      <c r="D41" s="144"/>
-      <c r="E41" s="144"/>
-      <c r="F41" s="144"/>
-      <c r="G41" s="144"/>
-      <c r="H41" s="144"/>
-      <c r="I41" s="144"/>
-      <c r="J41" s="144"/>
-      <c r="K41" s="144"/>
-      <c r="L41" s="144"/>
-      <c r="M41" s="144"/>
-      <c r="N41" s="144"/>
-    </row>
-    <row r="42" spans="2:14">
-      <c r="B42" s="143"/>
-      <c r="C42" s="144" t="s">
-        <v>145</v>
-      </c>
-      <c r="D42" s="144"/>
-      <c r="E42" s="144"/>
-      <c r="F42" s="144"/>
-      <c r="G42" s="144"/>
-      <c r="H42" s="144"/>
-      <c r="I42" s="144"/>
-      <c r="J42" s="144"/>
-      <c r="K42" s="144"/>
-      <c r="L42" s="144"/>
-      <c r="M42" s="144"/>
-      <c r="N42" s="144"/>
-    </row>
-    <row r="43" spans="2:14">
-      <c r="B43" s="143"/>
-      <c r="C43" s="144" t="s">
-        <v>146</v>
-      </c>
-      <c r="D43" s="144"/>
-      <c r="E43" s="144"/>
-      <c r="F43" s="144"/>
-      <c r="G43" s="144"/>
-      <c r="H43" s="144"/>
-      <c r="I43" s="144"/>
-      <c r="J43" s="144"/>
-      <c r="K43" s="144"/>
-      <c r="L43" s="144"/>
-      <c r="M43" s="144"/>
-      <c r="N43" s="144"/>
-    </row>
-    <row r="44" spans="2:14">
-      <c r="B44" s="143"/>
-      <c r="C44" s="144"/>
-      <c r="D44" s="144"/>
-      <c r="E44" s="144"/>
-      <c r="F44" s="144"/>
-      <c r="G44" s="144"/>
-      <c r="H44" s="144"/>
-      <c r="I44" s="144"/>
-      <c r="J44" s="144"/>
-      <c r="K44" s="144"/>
-      <c r="L44" s="144"/>
-      <c r="M44" s="144"/>
-      <c r="N44" s="144"/>
-    </row>
-    <row r="45" spans="2:14">
-      <c r="B45" s="143"/>
-      <c r="C45" s="144"/>
-      <c r="D45" s="144"/>
-      <c r="E45" s="144"/>
-      <c r="F45" s="144"/>
-      <c r="G45" s="144"/>
-      <c r="H45" s="144"/>
-      <c r="I45" s="144"/>
-      <c r="J45" s="144"/>
-      <c r="K45" s="144"/>
-      <c r="L45" s="144"/>
-      <c r="M45" s="144"/>
-      <c r="N45" s="144"/>
-    </row>
-    <row r="46" spans="2:14">
-      <c r="B46" s="143"/>
-      <c r="C46" s="144"/>
-      <c r="D46" s="144"/>
-      <c r="E46" s="144"/>
-      <c r="F46" s="144"/>
-      <c r="G46" s="144"/>
-      <c r="H46" s="144"/>
-      <c r="I46" s="144"/>
-      <c r="J46" s="144"/>
-      <c r="K46" s="144"/>
-      <c r="L46" s="144"/>
-      <c r="M46" s="144"/>
-      <c r="N46" s="144"/>
-    </row>
-    <row r="47" spans="2:14">
-      <c r="B47" s="143"/>
-      <c r="C47" s="144"/>
-      <c r="D47" s="144"/>
-      <c r="E47" s="144">
-        <v>2.5</v>
-      </c>
-      <c r="F47" s="144" t="s">
-        <v>149</v>
-      </c>
-      <c r="G47" s="144"/>
-      <c r="H47" s="144"/>
-      <c r="I47" s="144"/>
-      <c r="J47" s="144"/>
-      <c r="K47" s="144"/>
-      <c r="L47" s="144"/>
-      <c r="M47" s="144"/>
-      <c r="N47" s="144"/>
-    </row>
-    <row r="48" spans="2:14">
-      <c r="B48" s="143"/>
-      <c r="C48" s="144"/>
-      <c r="D48" s="144"/>
-      <c r="E48" s="144"/>
-      <c r="F48" s="144"/>
-      <c r="G48" s="144"/>
-      <c r="H48" s="144"/>
-      <c r="I48" s="144"/>
-      <c r="J48" s="144"/>
-      <c r="K48" s="144"/>
-      <c r="L48" s="144"/>
-      <c r="M48" s="144"/>
-      <c r="N48" s="144"/>
-    </row>
-    <row r="49" spans="2:14">
-      <c r="B49" s="143"/>
-      <c r="C49" s="144"/>
-      <c r="D49" s="144"/>
-      <c r="E49" s="144"/>
-      <c r="F49" s="144"/>
-      <c r="G49" s="144"/>
-      <c r="H49" s="144"/>
-      <c r="I49" s="144"/>
-      <c r="J49" s="144"/>
-      <c r="K49" s="144"/>
-      <c r="L49" s="144"/>
-      <c r="M49" s="144"/>
-      <c r="N49" s="144"/>
-    </row>
-    <row r="50" spans="2:14">
-      <c r="B50" s="143"/>
-      <c r="C50" s="144"/>
-      <c r="D50" s="144"/>
-      <c r="E50" s="144"/>
-      <c r="F50" s="144"/>
-      <c r="G50" s="144"/>
-      <c r="H50" s="144"/>
-      <c r="I50" s="144"/>
-      <c r="J50" s="144"/>
-      <c r="K50" s="144"/>
-      <c r="L50" s="144"/>
-      <c r="M50" s="144"/>
-      <c r="N50" s="144"/>
-    </row>
-    <row r="51" spans="2:14">
-      <c r="B51" s="143"/>
-      <c r="C51" s="144"/>
-      <c r="D51" s="144"/>
-      <c r="E51" s="144"/>
-      <c r="F51" s="144"/>
-      <c r="G51" s="144"/>
-      <c r="H51" s="144"/>
-      <c r="I51" s="144"/>
-      <c r="J51" s="144"/>
-      <c r="K51" s="144"/>
-      <c r="L51" s="144"/>
-      <c r="M51" s="144"/>
-      <c r="N51" s="144"/>
-    </row>
-    <row r="52" spans="2:14">
-      <c r="B52" s="143"/>
-      <c r="C52" s="144"/>
-      <c r="D52" s="144"/>
-      <c r="E52" s="144"/>
-      <c r="F52" s="144"/>
-      <c r="G52" s="144"/>
-      <c r="H52" s="144"/>
-      <c r="I52" s="144"/>
-      <c r="J52" s="144"/>
-      <c r="K52" s="144"/>
-      <c r="L52" s="144"/>
-      <c r="M52" s="144"/>
-      <c r="N52" s="144"/>
-    </row>
-    <row r="53" spans="2:14">
-      <c r="B53" s="143"/>
-      <c r="C53" s="144"/>
-      <c r="D53" s="144"/>
-      <c r="E53" s="144">
-        <v>20</v>
-      </c>
-      <c r="F53" s="144" t="s">
-        <v>149</v>
-      </c>
-      <c r="G53" s="144"/>
-      <c r="H53" s="144"/>
-      <c r="I53" s="144"/>
-      <c r="J53" s="144"/>
-      <c r="K53" s="144"/>
-      <c r="L53" s="144"/>
-      <c r="M53" s="144"/>
-      <c r="N53" s="144"/>
-    </row>
-    <row r="54" spans="2:14">
-      <c r="B54" s="143"/>
-      <c r="C54" s="144"/>
-      <c r="D54" s="144"/>
-      <c r="E54" s="144"/>
-      <c r="F54" s="144"/>
-      <c r="G54" s="144"/>
-      <c r="H54" s="144"/>
-      <c r="I54" s="144"/>
-      <c r="J54" s="144"/>
-      <c r="K54" s="144"/>
-      <c r="L54" s="144"/>
-      <c r="M54" s="144"/>
-      <c r="N54" s="144"/>
-    </row>
-    <row r="55" spans="2:14">
-      <c r="B55" s="143"/>
-      <c r="C55" s="144"/>
-      <c r="D55" s="144"/>
-      <c r="E55" s="144"/>
-      <c r="F55" s="144"/>
-      <c r="G55" s="144"/>
-      <c r="H55" s="144"/>
-      <c r="I55" s="144"/>
-      <c r="J55" s="144"/>
-      <c r="K55" s="144"/>
-      <c r="L55" s="144"/>
-      <c r="M55" s="144"/>
-      <c r="N55" s="144"/>
-    </row>
-    <row r="56" spans="2:14">
-      <c r="B56" s="143"/>
-      <c r="C56" s="144"/>
-      <c r="D56" s="144"/>
-      <c r="E56" s="144"/>
-      <c r="F56" s="144"/>
-      <c r="G56" s="144"/>
-      <c r="H56" s="144"/>
-      <c r="I56" s="144"/>
-      <c r="J56" s="144"/>
-      <c r="K56" s="144"/>
-      <c r="L56" s="144"/>
-      <c r="M56" s="144"/>
-      <c r="N56" s="144"/>
-    </row>
-    <row r="57" spans="2:14">
-      <c r="B57" s="143"/>
-      <c r="C57" s="144"/>
-      <c r="D57" s="144"/>
-      <c r="E57" s="144"/>
-      <c r="F57" s="144"/>
-      <c r="G57" s="144"/>
-      <c r="H57" s="144"/>
-      <c r="I57" s="144"/>
-      <c r="J57" s="144"/>
-      <c r="K57" s="144"/>
-      <c r="L57" s="144"/>
-      <c r="M57" s="144"/>
-      <c r="N57" s="144"/>
-    </row>
-    <row r="58" spans="2:14">
-      <c r="B58" s="143"/>
-      <c r="C58" s="144"/>
-      <c r="D58" s="144"/>
-      <c r="E58" s="144"/>
-      <c r="F58" s="144"/>
-      <c r="G58" s="144"/>
-      <c r="H58" s="144"/>
-      <c r="I58" s="144"/>
-      <c r="J58" s="144"/>
-      <c r="K58" s="144"/>
-      <c r="L58" s="144"/>
-      <c r="M58" s="144"/>
-      <c r="N58" s="144"/>
-    </row>
-    <row r="59" spans="2:14">
-      <c r="B59" s="143"/>
-      <c r="C59" s="144"/>
-      <c r="D59" s="144"/>
-      <c r="E59" s="144"/>
-      <c r="F59" s="144"/>
-      <c r="G59" s="144"/>
-      <c r="H59" s="144"/>
-      <c r="I59" s="144"/>
-      <c r="J59" s="144"/>
-      <c r="K59" s="144"/>
-      <c r="L59" s="144"/>
-      <c r="M59" s="144"/>
-      <c r="N59" s="144"/>
-    </row>
-    <row r="60" spans="2:14">
-      <c r="B60" s="143"/>
-      <c r="C60" s="144"/>
-      <c r="D60" s="144"/>
-      <c r="E60" s="144"/>
-      <c r="F60" s="144"/>
-      <c r="G60" s="144"/>
-      <c r="H60" s="144"/>
-      <c r="I60" s="144"/>
-      <c r="J60" s="144"/>
-      <c r="K60" s="144"/>
-      <c r="L60" s="144"/>
-      <c r="M60" s="144"/>
-      <c r="N60" s="144"/>
-    </row>
-    <row r="61" spans="2:14">
-      <c r="B61" s="143"/>
-      <c r="C61" s="144" t="s">
-        <v>147</v>
-      </c>
-      <c r="D61" s="144"/>
-      <c r="E61" s="144"/>
-      <c r="F61" s="144"/>
-      <c r="G61" s="144"/>
-      <c r="H61" s="144"/>
-      <c r="I61" s="144"/>
-      <c r="J61" s="144"/>
-      <c r="K61" s="144"/>
-      <c r="L61" s="144"/>
-      <c r="M61" s="144"/>
-      <c r="N61" s="144"/>
-    </row>
-    <row r="62" spans="2:14">
-      <c r="B62" s="143"/>
-      <c r="C62" s="144" t="s">
-        <v>148</v>
-      </c>
-      <c r="D62" s="144"/>
-      <c r="E62" s="144"/>
-      <c r="F62" s="144"/>
-      <c r="G62" s="144"/>
-      <c r="H62" s="144"/>
-      <c r="I62" s="144"/>
-      <c r="J62" s="144"/>
-      <c r="K62" s="144"/>
-      <c r="L62" s="144"/>
-      <c r="M62" s="144"/>
-      <c r="N62" s="144"/>
-    </row>
-    <row r="63" spans="2:14">
-      <c r="B63" s="143"/>
-      <c r="C63" s="144"/>
-      <c r="D63" s="144"/>
-      <c r="E63" s="144"/>
-      <c r="F63" s="144"/>
-      <c r="G63" s="144"/>
-      <c r="H63" s="144"/>
-      <c r="I63" s="144"/>
-      <c r="J63" s="144"/>
-      <c r="K63" s="144"/>
-      <c r="L63" s="144"/>
-      <c r="M63" s="144"/>
-      <c r="N63" s="144"/>
-    </row>
-    <row r="64" spans="2:14">
-      <c r="B64" s="143"/>
-      <c r="C64" s="144"/>
-      <c r="D64" s="144"/>
-      <c r="E64" s="144"/>
-      <c r="F64" s="144"/>
-      <c r="G64" s="144"/>
-      <c r="H64" s="144"/>
-      <c r="I64" s="144"/>
-      <c r="J64" s="144"/>
-      <c r="K64" s="144"/>
-      <c r="L64" s="144"/>
-      <c r="M64" s="144"/>
-      <c r="N64" s="144"/>
-    </row>
-    <row r="65" spans="2:14">
-      <c r="B65" s="143"/>
-      <c r="C65" s="144"/>
-      <c r="D65" s="144"/>
-      <c r="E65" s="144"/>
-      <c r="F65" s="144"/>
-      <c r="G65" s="144"/>
-      <c r="H65" s="144"/>
-      <c r="I65" s="144"/>
-      <c r="J65" s="144"/>
-      <c r="K65" s="144"/>
-      <c r="L65" s="144"/>
-      <c r="M65" s="144"/>
-      <c r="N65" s="144"/>
-    </row>
-    <row r="66" spans="2:14">
-      <c r="B66" s="143"/>
-      <c r="C66" s="144"/>
-      <c r="D66" s="144"/>
-      <c r="E66" s="144"/>
-      <c r="F66" s="144"/>
-      <c r="G66" s="144"/>
-      <c r="H66" s="144"/>
-      <c r="I66" s="144"/>
-      <c r="J66" s="144"/>
-      <c r="K66" s="144"/>
-      <c r="L66" s="144"/>
-      <c r="M66" s="144"/>
-      <c r="N66" s="144"/>
-    </row>
-    <row r="67" spans="2:14">
-      <c r="B67" s="143"/>
-      <c r="C67" s="144"/>
-      <c r="D67" s="144"/>
-      <c r="E67" s="144"/>
-      <c r="F67" s="144"/>
-      <c r="G67" s="144"/>
-      <c r="H67" s="144"/>
-      <c r="I67" s="144"/>
-      <c r="J67" s="144"/>
-      <c r="K67" s="144"/>
-      <c r="L67" s="144"/>
-      <c r="M67" s="144"/>
-      <c r="N67" s="144"/>
-    </row>
-    <row r="68" spans="2:14">
-      <c r="B68" s="143"/>
-      <c r="C68" s="144"/>
-      <c r="D68" s="144"/>
-      <c r="E68" s="144"/>
-      <c r="F68" s="144"/>
-      <c r="G68" s="144"/>
-      <c r="H68" s="144"/>
-      <c r="I68" s="144"/>
-      <c r="J68" s="144"/>
-      <c r="K68" s="144"/>
-      <c r="L68" s="144"/>
-      <c r="M68" s="144"/>
-      <c r="N68" s="144"/>
-    </row>
-    <row r="69" spans="2:14">
-      <c r="B69" s="143"/>
-      <c r="C69" s="144"/>
-      <c r="D69" s="144"/>
-      <c r="E69" s="144"/>
-      <c r="F69" s="144"/>
-      <c r="G69" s="144"/>
-      <c r="H69" s="144"/>
-      <c r="I69" s="144"/>
-      <c r="J69" s="144"/>
-      <c r="K69" s="144"/>
-      <c r="L69" s="144"/>
-      <c r="M69" s="144"/>
-      <c r="N69" s="144"/>
-    </row>
-    <row r="70" spans="2:14">
-      <c r="B70" s="143"/>
-      <c r="C70" s="144"/>
-      <c r="D70" s="144"/>
-      <c r="E70" s="144">
-        <v>30</v>
-      </c>
-      <c r="F70" s="144" t="s">
-        <v>149</v>
-      </c>
-      <c r="G70" s="144"/>
-      <c r="H70" s="144"/>
-      <c r="I70" s="144"/>
-      <c r="J70" s="144"/>
-      <c r="K70" s="144"/>
-      <c r="L70" s="144"/>
-      <c r="M70" s="144"/>
-      <c r="N70" s="144"/>
+      <c r="G70" s="138"/>
+      <c r="H70" s="138"/>
+      <c r="I70" s="138"/>
+      <c r="J70" s="138"/>
+      <c r="K70" s="138"/>
+      <c r="L70" s="138"/>
+      <c r="M70" s="138"/>
+      <c r="N70" s="138"/>
     </row>
     <row r="71" spans="2:14">
-      <c r="B71" s="143"/>
-      <c r="C71" s="144"/>
-      <c r="D71" s="144"/>
-      <c r="E71" s="144"/>
-      <c r="F71" s="144"/>
-      <c r="G71" s="144"/>
-      <c r="H71" s="144"/>
-      <c r="I71" s="144"/>
-      <c r="J71" s="144"/>
-      <c r="K71" s="144"/>
-      <c r="L71" s="144"/>
-      <c r="M71" s="144"/>
-      <c r="N71" s="144"/>
+      <c r="B71" s="137"/>
+      <c r="C71" s="138"/>
+      <c r="D71" s="138"/>
+      <c r="E71" s="138"/>
+      <c r="F71" s="138"/>
+      <c r="G71" s="138"/>
+      <c r="H71" s="138"/>
+      <c r="I71" s="138"/>
+      <c r="J71" s="138"/>
+      <c r="K71" s="138"/>
+      <c r="L71" s="138"/>
+      <c r="M71" s="138"/>
+      <c r="N71" s="138"/>
     </row>
     <row r="72" spans="2:14">
-      <c r="B72" s="143"/>
-      <c r="C72" s="144"/>
-      <c r="D72" s="144"/>
-      <c r="E72" s="144"/>
-      <c r="F72" s="144"/>
-      <c r="G72" s="144"/>
-      <c r="H72" s="144"/>
-      <c r="I72" s="144"/>
-      <c r="J72" s="144"/>
-      <c r="K72" s="144"/>
-      <c r="L72" s="144"/>
-      <c r="M72" s="144"/>
-      <c r="N72" s="144"/>
+      <c r="B72" s="137"/>
+      <c r="C72" s="138"/>
+      <c r="D72" s="138"/>
+      <c r="E72" s="138"/>
+      <c r="F72" s="138"/>
+      <c r="G72" s="138"/>
+      <c r="H72" s="138"/>
+      <c r="I72" s="138"/>
+      <c r="J72" s="138"/>
+      <c r="K72" s="138"/>
+      <c r="L72" s="138"/>
+      <c r="M72" s="138"/>
+      <c r="N72" s="138"/>
     </row>
     <row r="73" spans="2:14">
-      <c r="B73" s="143"/>
-      <c r="C73" s="144"/>
-      <c r="D73" s="144"/>
-      <c r="E73" s="144"/>
-      <c r="F73" s="144"/>
-      <c r="G73" s="144"/>
-      <c r="H73" s="144"/>
-      <c r="I73" s="144"/>
-      <c r="J73" s="144"/>
-      <c r="K73" s="144"/>
-      <c r="L73" s="144"/>
-      <c r="M73" s="144"/>
-      <c r="N73" s="144"/>
+      <c r="B73" s="137"/>
+      <c r="C73" s="138"/>
+      <c r="D73" s="138"/>
+      <c r="E73" s="138"/>
+      <c r="F73" s="138"/>
+      <c r="G73" s="138"/>
+      <c r="H73" s="138"/>
+      <c r="I73" s="138"/>
+      <c r="J73" s="138"/>
+      <c r="K73" s="138"/>
+      <c r="L73" s="138"/>
+      <c r="M73" s="138"/>
+      <c r="N73" s="138"/>
     </row>
     <row r="74" spans="2:14">
-      <c r="B74" s="143"/>
-      <c r="C74" s="144"/>
-      <c r="D74" s="144"/>
-      <c r="E74" s="144"/>
-      <c r="F74" s="144"/>
-      <c r="G74" s="144"/>
-      <c r="H74" s="144"/>
-      <c r="I74" s="144"/>
-      <c r="J74" s="144"/>
-      <c r="K74" s="144"/>
-      <c r="L74" s="144"/>
-      <c r="M74" s="144"/>
-      <c r="N74" s="144"/>
+      <c r="B74" s="137"/>
+      <c r="C74" s="138"/>
+      <c r="D74" s="138"/>
+      <c r="E74" s="138"/>
+      <c r="F74" s="138"/>
+      <c r="G74" s="138"/>
+      <c r="H74" s="138"/>
+      <c r="I74" s="138"/>
+      <c r="J74" s="138"/>
+      <c r="K74" s="138"/>
+      <c r="L74" s="138"/>
+      <c r="M74" s="138"/>
+      <c r="N74" s="138"/>
     </row>
     <row r="75" spans="2:14">
-      <c r="B75" s="143"/>
-      <c r="C75" s="144"/>
-      <c r="D75" s="144"/>
-      <c r="E75" s="144"/>
-      <c r="F75" s="144"/>
-      <c r="G75" s="144"/>
-      <c r="H75" s="144"/>
-      <c r="I75" s="144"/>
-      <c r="J75" s="144"/>
-      <c r="K75" s="144"/>
-      <c r="L75" s="144"/>
-      <c r="M75" s="144"/>
-      <c r="N75" s="144"/>
+      <c r="B75" s="137"/>
+      <c r="C75" s="138"/>
+      <c r="D75" s="138"/>
+      <c r="E75" s="138"/>
+      <c r="F75" s="138"/>
+      <c r="G75" s="138"/>
+      <c r="H75" s="138"/>
+      <c r="I75" s="138"/>
+      <c r="J75" s="138"/>
+      <c r="K75" s="138"/>
+      <c r="L75" s="138"/>
+      <c r="M75" s="138"/>
+      <c r="N75" s="138"/>
     </row>
     <row r="76" spans="2:14">
-      <c r="B76" s="143"/>
-      <c r="C76" s="144"/>
-      <c r="D76" s="144"/>
-      <c r="E76" s="144"/>
-      <c r="F76" s="144"/>
-      <c r="G76" s="144"/>
-      <c r="H76" s="144"/>
-      <c r="I76" s="144"/>
-      <c r="J76" s="144"/>
-      <c r="K76" s="144"/>
-      <c r="L76" s="144"/>
-      <c r="M76" s="144"/>
-      <c r="N76" s="144"/>
+      <c r="B76" s="137"/>
+      <c r="C76" s="138"/>
+      <c r="D76" s="138"/>
+      <c r="E76" s="138"/>
+      <c r="F76" s="138"/>
+      <c r="G76" s="138"/>
+      <c r="H76" s="138"/>
+      <c r="I76" s="138"/>
+      <c r="J76" s="138"/>
+      <c r="K76" s="138"/>
+      <c r="L76" s="138"/>
+      <c r="M76" s="138"/>
+      <c r="N76" s="138"/>
     </row>
     <row r="77" spans="2:14">
-      <c r="B77" s="143"/>
-      <c r="C77" s="144"/>
-      <c r="D77" s="144"/>
-      <c r="E77" s="144"/>
-      <c r="F77" s="144"/>
-      <c r="G77" s="144"/>
-      <c r="H77" s="144"/>
-      <c r="I77" s="144"/>
-      <c r="J77" s="144"/>
-      <c r="K77" s="144"/>
-      <c r="L77" s="144"/>
-      <c r="M77" s="144"/>
-      <c r="N77" s="144"/>
+      <c r="B77" s="137"/>
+      <c r="C77" s="138"/>
+      <c r="D77" s="138"/>
+      <c r="E77" s="138"/>
+      <c r="F77" s="138"/>
+      <c r="G77" s="138"/>
+      <c r="H77" s="138"/>
+      <c r="I77" s="138"/>
+      <c r="J77" s="138"/>
+      <c r="K77" s="138"/>
+      <c r="L77" s="138"/>
+      <c r="M77" s="138"/>
+      <c r="N77" s="138"/>
     </row>
     <row r="78" spans="2:14">
-      <c r="B78" s="143"/>
-      <c r="C78" s="144"/>
-      <c r="D78" s="144"/>
-      <c r="E78" s="144"/>
-      <c r="F78" s="144"/>
-      <c r="G78" s="144"/>
-      <c r="H78" s="144"/>
-      <c r="I78" s="144"/>
-      <c r="J78" s="144"/>
-      <c r="K78" s="144"/>
-      <c r="L78" s="144"/>
-      <c r="M78" s="144"/>
-      <c r="N78" s="144"/>
+      <c r="B78" s="137"/>
+      <c r="C78" s="138"/>
+      <c r="D78" s="138"/>
+      <c r="E78" s="138"/>
+      <c r="F78" s="138"/>
+      <c r="G78" s="138"/>
+      <c r="H78" s="138"/>
+      <c r="I78" s="138"/>
+      <c r="J78" s="138"/>
+      <c r="K78" s="138"/>
+      <c r="L78" s="138"/>
+      <c r="M78" s="138"/>
+      <c r="N78" s="138"/>
     </row>
     <row r="79" spans="2:14">
-      <c r="B79" s="143"/>
-      <c r="C79" s="144"/>
-      <c r="D79" s="144"/>
-      <c r="E79" s="144"/>
-      <c r="F79" s="144"/>
-      <c r="G79" s="144"/>
-      <c r="H79" s="144"/>
-      <c r="I79" s="144"/>
-      <c r="J79" s="144"/>
-      <c r="K79" s="144"/>
-      <c r="L79" s="144"/>
-      <c r="M79" s="144"/>
-      <c r="N79" s="144"/>
+      <c r="B79" s="137"/>
+      <c r="C79" s="138"/>
+      <c r="D79" s="138"/>
+      <c r="E79" s="138"/>
+      <c r="F79" s="138"/>
+      <c r="G79" s="138"/>
+      <c r="H79" s="138"/>
+      <c r="I79" s="138"/>
+      <c r="J79" s="138"/>
+      <c r="K79" s="138"/>
+      <c r="L79" s="138"/>
+      <c r="M79" s="138"/>
+      <c r="N79" s="138"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>